<commit_message>
added comm mission points display, made toggle-able
</commit_message>
<xml_diff>
--- a/SatManager Work Breakdown Structure.xlsx
+++ b/SatManager Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>Status</t>
   </si>
@@ -366,6 +366,9 @@
     <t xml:space="preserve">initialize points</t>
   </si>
   <si>
+    <t xml:space="preserve">display points</t>
+  </si>
+  <si>
     <t>reward</t>
   </si>
   <si>
@@ -396,6 +399,9 @@
     <t>rendevous</t>
   </si>
   <si>
+    <t xml:space="preserve">selected mission details</t>
+  </si>
+  <si>
     <t xml:space="preserve">available missions</t>
   </si>
   <si>
@@ -405,7 +411,7 @@
     <t xml:space="preserve">select to view parameters</t>
   </si>
   <si>
-    <t xml:space="preserve">show points when selected</t>
+    <t xml:space="preserve">highlight points when selected</t>
   </si>
   <si>
     <t xml:space="preserve">show reward</t>
@@ -591,7 +597,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -633,6 +639,9 @@
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -660,7 +669,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J129" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J131" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1170,7 +1179,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A94" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A76" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1225,13 +1234,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.3203125</v>
+        <v>0.33846153846153848</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I124,"0")/ROWS(Table5[])</f>
-        <v>2.34375e-002</v>
+        <f>COUNTIF(I2:I126,"0")/ROWS(Table5[])</f>
+        <v>2.3076923076923078e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1268,7 +1277,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1303,7 +1312,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -2520,7 +2529,9 @@
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
-      <c r="I84" s="6"/>
+      <c r="I84" s="6">
+        <v>0</v>
+      </c>
       <c r="J84" s="9"/>
     </row>
     <row r="85" ht="14.25">
@@ -2595,7 +2606,7 @@
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
-      <c r="F89" s="4" t="s">
+      <c r="F89" s="15" t="s">
         <v>117</v>
       </c>
       <c r="G89" s="4"/>
@@ -2616,7 +2627,9 @@
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
-      <c r="I90" s="6"/>
+      <c r="I90" s="6">
+        <v>1</v>
+      </c>
       <c r="J90" s="9"/>
     </row>
     <row r="91" ht="14.25">
@@ -2624,32 +2637,30 @@
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
-      <c r="E91" s="4" t="s">
+      <c r="E91" s="4"/>
+      <c r="F91" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F91" s="4"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="6"/>
-      <c r="J91" s="9" t="s">
-        <v>120</v>
-      </c>
+      <c r="J91" s="9"/>
     </row>
     <row r="92" ht="14.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4" t="s">
-        <v>121</v>
-      </c>
+      <c r="E92" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
-      <c r="I92" s="6">
-        <v>1</v>
-      </c>
-      <c r="J92" s="9"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="9" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="93" ht="14.25">
       <c r="A93" s="4"/>
@@ -2658,7 +2669,7 @@
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -2678,7 +2689,9 @@
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
-      <c r="I94" s="6"/>
+      <c r="I94" s="6">
+        <v>1</v>
+      </c>
       <c r="J94" s="9"/>
     </row>
     <row r="95" ht="14.25">
@@ -2686,10 +2699,10 @@
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
-      <c r="E95" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="6"/>
@@ -2700,10 +2713,10 @@
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="4" t="s">
+      <c r="E96" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="F96" s="4"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="6"/>
@@ -2716,7 +2729,7 @@
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
@@ -2742,10 +2755,10 @@
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F99" s="4"/>
+      <c r="E99" s="4"/>
+      <c r="F99" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="6"/>
@@ -2756,10 +2769,10 @@
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4" t="s">
-        <v>124</v>
-      </c>
+      <c r="E100" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F100" s="4"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="6"/>
@@ -2772,7 +2785,7 @@
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
       <c r="F101" s="4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
@@ -2798,10 +2811,10 @@
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
-      <c r="E103" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="F103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="6"/>
@@ -2812,10 +2825,10 @@
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4" t="s">
-        <v>123</v>
-      </c>
+      <c r="E104" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="6"/>
@@ -2828,7 +2841,7 @@
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
@@ -2850,46 +2863,46 @@
       <c r="J106" s="9"/>
     </row>
     <row r="107" ht="14.25">
-      <c r="A107" s="11"/>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="F107" s="11"/>
-      <c r="G107" s="11"/>
-      <c r="H107" s="11"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="10"/>
+      <c r="A107" s="4"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="9"/>
     </row>
     <row r="108" ht="14.25">
       <c r="A108" s="11"/>
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
       <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
-      <c r="F108" s="11" t="s">
-        <v>123</v>
-      </c>
+      <c r="E108" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F108" s="11"/>
       <c r="G108" s="11"/>
       <c r="H108" s="11"/>
       <c r="I108" s="13"/>
       <c r="J108" s="10"/>
     </row>
     <row r="109" ht="14.25">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G109" s="4"/>
-      <c r="H109" s="4"/>
-      <c r="I109" s="6"/>
-      <c r="J109" s="9"/>
+      <c r="A109" s="11"/>
+      <c r="B109" s="11"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G109" s="11"/>
+      <c r="H109" s="11"/>
+      <c r="I109" s="13"/>
+      <c r="J109" s="10"/>
     </row>
     <row r="110" ht="14.25">
       <c r="A110" s="4"/>
@@ -2909,26 +2922,24 @@
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
-      <c r="D111" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D111" s="4"/>
       <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
+      <c r="F111" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
-      <c r="I111" s="6">
-        <v>0</v>
-      </c>
+      <c r="I111" s="6"/>
       <c r="J111" s="9"/>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="D112" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" s="4"/>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
@@ -2942,15 +2953,13 @@
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
-      <c r="E113" s="4"/>
-      <c r="F113" s="4" t="s">
+      <c r="E113" s="15" t="s">
         <v>128</v>
       </c>
+      <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="6">
-        <v>0</v>
-      </c>
+      <c r="I113" s="6"/>
       <c r="J113" s="9"/>
     </row>
     <row r="114" ht="14.25">
@@ -2958,13 +2967,15 @@
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
-      <c r="E114" s="4"/>
-      <c r="F114" s="4" t="s">
+      <c r="E114" s="4" t="s">
         <v>129</v>
       </c>
+      <c r="F114" s="4"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
-      <c r="I114" s="6"/>
+      <c r="I114" s="6">
+        <v>0</v>
+      </c>
       <c r="J114" s="9"/>
     </row>
     <row r="115" ht="14.25">
@@ -2978,7 +2989,9 @@
       </c>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
-      <c r="I115" s="6"/>
+      <c r="I115" s="6">
+        <v>1</v>
+      </c>
       <c r="J115" s="9"/>
     </row>
     <row r="116" ht="14.25">
@@ -2999,11 +3012,11 @@
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
-      <c r="D117" s="4" t="s">
+      <c r="D117" s="4"/>
+      <c r="E117" s="4"/>
+      <c r="F117" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="E117" s="4"/>
-      <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="6">
@@ -3016,25 +3029,22 @@
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
-      <c r="E118" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F118" s="4"/>
+      <c r="F118" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
-      <c r="I118" s="6">
-        <v>1</v>
-      </c>
+      <c r="I118" s="6"/>
       <c r="J118" s="9"/>
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
-      <c r="E119" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="D119" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
@@ -3046,38 +3056,42 @@
     <row r="120" ht="14.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
-      <c r="C120" s="4" t="s">
-        <v>134</v>
-      </c>
+      <c r="C120" s="4"/>
       <c r="D120" s="4"/>
-      <c r="E120" s="4"/>
+      <c r="E120" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
-      <c r="I120" s="6"/>
+      <c r="I120" s="6">
+        <v>1</v>
+      </c>
       <c r="J120" s="9"/>
     </row>
     <row r="121" ht="14.25">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
-      <c r="D121" s="4" t="s">
+      <c r="D121" s="4"/>
+      <c r="E121" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="E121" s="4"/>
       <c r="F121" s="4"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
-      <c r="I121" s="6"/>
+      <c r="I121" s="6">
+        <v>1</v>
+      </c>
       <c r="J121" s="9"/>
     </row>
     <row r="122" ht="14.25">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4" t="s">
+      <c r="C122" s="4" t="s">
         <v>136</v>
       </c>
+      <c r="D122" s="4"/>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
       <c r="G122" s="4"/>
@@ -3104,7 +3118,7 @@
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4" t="s">
-        <v>20</v>
+        <v>138</v>
       </c>
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
@@ -3115,11 +3129,11 @@
     </row>
     <row r="125" ht="14.25">
       <c r="A125" s="4"/>
-      <c r="B125" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="B125" s="4"/>
       <c r="C125" s="4"/>
-      <c r="D125" s="4"/>
+      <c r="D125" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
       <c r="G125" s="4"/>
@@ -3130,62 +3144,90 @@
     <row r="126" ht="14.25">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
-      <c r="C126" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D126" s="4"/>
+      <c r="C126" s="4"/>
+      <c r="D126" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
       <c r="I126" s="6"/>
-      <c r="J126" s="9" t="s">
-        <v>139</v>
-      </c>
+      <c r="J126" s="9"/>
     </row>
     <row r="127" ht="14.25">
       <c r="A127" s="4"/>
-      <c r="B127" s="4"/>
-      <c r="C127" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>140</v>
       </c>
+      <c r="C127" s="4"/>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
       <c r="G127" s="4"/>
       <c r="H127" s="4"/>
       <c r="I127" s="6"/>
-      <c r="J127" s="9" t="s">
-        <v>141</v>
-      </c>
+      <c r="J127" s="9"/>
     </row>
     <row r="128" ht="14.25">
       <c r="A128" s="4"/>
-      <c r="B128" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C128" s="4"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
       <c r="G128" s="4"/>
-      <c r="H128" s="15"/>
+      <c r="H128" s="4"/>
       <c r="I128" s="6"/>
-      <c r="J128" s="16"/>
+      <c r="J128" s="9" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="129" ht="14.25">
-      <c r="C129" t="s">
+      <c r="A129" s="4"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D129" s="4"/>
+      <c r="E129" s="4"/>
+      <c r="F129" s="4"/>
+      <c r="G129" s="4"/>
+      <c r="H129" s="4"/>
+      <c r="I129" s="6"/>
+      <c r="J129" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="I129" s="6"/>
-      <c r="J129" t="s">
+    </row>
+    <row r="130" ht="14.25">
+      <c r="A130" s="4"/>
+      <c r="B130" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="130" ht="14.25">
-      <c r="C130" s="17"/>
-      <c r="I130" s="4"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="4"/>
+      <c r="E130" s="4"/>
+      <c r="F130" s="4"/>
+      <c r="G130" s="4"/>
+      <c r="H130" s="16"/>
+      <c r="I130" s="6"/>
       <c r="J130" s="17"/>
+    </row>
+    <row r="131" ht="14.25">
+      <c r="C131" t="s">
+        <v>145</v>
+      </c>
+      <c r="I131" s="6"/>
+      <c r="J131" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="132" ht="14.25">
+      <c r="C132" s="18"/>
+      <c r="I132" s="4"/>
+      <c r="J132" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3205,7 +3247,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00F700BD-004D-4F8A-AB45-0012000400E3}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00ED00D2-00B9-44D5-820E-00A700CB0039}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3219,10 +3261,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I111 I112:I124 I46:I49</xm:sqref>
+          <xm:sqref>I3:I112 I114:I126 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00CA0013-0027-4E53-917D-00C800E8009A}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00720070-0016-435B-859D-006400120058}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3236,10 +3278,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I126</xm:sqref>
+          <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00F30013-00BF-48C3-B612-001100D20021}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E700EF-0089-4E2B-8B14-004500EF002C}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3253,10 +3295,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I125</xm:sqref>
+          <xm:sqref>I127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00180005-0027-49AA-B4EE-00C900A200AC}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00060092-0028-4FBD-BBCC-000100A40073}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3273,7 +3315,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00460067-00B6-4B6A-8A16-00C3003E00C5}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{002C000F-0089-4660-AA7F-008600B80082}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3290,7 +3332,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{006C0066-0088-487B-AC3B-0045000E00C9}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00DA000F-004B-4CB4-B5CE-0072007500BF}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3307,7 +3349,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00DD0069-00F9-4BE8-B72C-0089007E0068}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003800B1-008E-422F-BABC-009C006A0026}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3324,7 +3366,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D20086-002E-41D0-A662-003E00800028}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{008D0007-0076-4399-9730-008900E900C4}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3341,7 +3383,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E6000B-008D-47E5-9F73-0005000800E2}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00C80097-00AC-438F-BC78-00F7008A003F}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3358,7 +3400,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{009800F6-003F-4DF1-8C9F-00F5008E0044}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00FB00DB-00DC-4304-91C1-005500A6004C}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3375,7 +3417,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00CD007D-00B5-464C-8747-0018008F004D}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00DA00C1-0038-49BC-A69F-004900DD0037}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3389,10 +3431,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I128</xm:sqref>
+          <xm:sqref>I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{004B0088-0020-4667-9271-00EB000B00D4}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0040002C-00F3-4ECF-B58D-00290091005F}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3406,10 +3448,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I129</xm:sqref>
+          <xm:sqref>I131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003F0031-00F7-4745-A544-00E100080002}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00AB0072-00C7-412C-B661-0082006800B8}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3426,7 +3468,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B7004B-0075-45FC-8592-00E1000F00D3}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00BB00DC-0070-4013-80DF-009500CE0047}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3440,10 +3482,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I126</xm:sqref>
+          <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{002900D8-0019-4438-B24A-00C300AA009A}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B70029-002F-4399-BF29-00D4007000A9}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3457,10 +3499,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I111 I112:I124 I46:I49</xm:sqref>
+          <xm:sqref>I3:I112 I114:I126 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00EB0091-0024-48B9-9E01-00D700EC007A}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0007000B-0048-4528-B048-006A00C3008C}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3477,7 +3519,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B90062-001E-4FD0-B972-005E00E900ED}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00BB00A9-0085-47FD-BAA5-00B0007B0034}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3491,10 +3533,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I125</xm:sqref>
+          <xm:sqref>I127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003200EB-0052-4BE5-8DFA-000F00390040}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0003001B-00B0-41A8-8E91-00B8001400F8}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3511,7 +3553,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{005A0001-004D-45F4-A81C-009400790015}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B500F1-001C-4290-98C0-00C6004D00C2}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3528,7 +3570,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{001A002B-0063-4E0C-91FB-000A00CB00E0}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00CB00AC-001D-4E6C-84CA-00D200A70093}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3545,7 +3587,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00BC0025-002A-4BCF-9DE2-00850051006A}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00E20042-008B-44CB-8FA8-000800EA00FD}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3562,7 +3604,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{006F0060-00FD-4EF5-80C0-008900B50052}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00BC009F-0044-498D-AA3E-004800A100A6}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3579,7 +3621,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C90080-007A-4FC8-BCA6-009200A40087}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00BE001F-00A7-4D67-ABCC-00A7009900CC}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3593,10 +3635,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I128</xm:sqref>
+          <xm:sqref>I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{004000DD-0005-4FA9-9B47-008D004E00CF}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00720015-0019-4663-947A-00EB006600BB}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3610,10 +3652,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I129</xm:sqref>
+          <xm:sqref>I131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00B00003-0043-4989-B880-005D00E90043}">
+          <x14:cfRule type="dataBar" priority="2" id="{00060048-0084-485D-9FD6-001300DE0059}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3629,7 +3671,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00D80032-009F-4271-9CCD-0057002B00D0}">
+          <x14:cfRule type="dataBar" priority="1" id="{00CC0070-00D3-4D88-A74E-00CD009C009B}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
Created mission details window, comm missions integrated
</commit_message>
<xml_diff>
--- a/SatManager Work Breakdown Structure.xlsx
+++ b/SatManager Work Breakdown Structure.xlsx
@@ -288,7 +288,7 @@
     <t xml:space="preserve">view health</t>
   </si>
   <si>
-    <t xml:space="preserve">fuel level, battery, etc.</t>
+    <t xml:space="preserve">fuel level, other health as added</t>
   </si>
   <si>
     <t xml:space="preserve">satellite motion</t>
@@ -636,10 +636,10 @@
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1179,7 +1179,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1234,13 +1234,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.33846153846153848</v>
+        <v>0.35384615384615387</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f>COUNTIF(I2:I126,"0")/ROWS(Table5[])</f>
-        <v>2.3076923076923078e-002</v>
+        <v>1.5384615384615385e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1312,7 +1312,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -2231,8 +2231,10 @@
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
-      <c r="I64" s="6"/>
-      <c r="J64" s="9" t="s">
+      <c r="I64" s="6">
+        <v>1</v>
+      </c>
+      <c r="J64" s="14" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2247,7 +2249,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="14">
+      <c r="I65" s="15">
         <v>1</v>
       </c>
       <c r="J65" s="9"/>
@@ -2263,7 +2265,9 @@
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
-      <c r="I66" s="6"/>
+      <c r="I66" s="6">
+        <v>1</v>
+      </c>
       <c r="J66" s="9"/>
     </row>
     <row r="67" ht="14.25">
@@ -2529,9 +2533,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
-      <c r="I84" s="6">
-        <v>0</v>
-      </c>
+      <c r="I84" s="6"/>
       <c r="J84" s="9"/>
     </row>
     <row r="85" ht="14.25">
@@ -2606,7 +2608,7 @@
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
-      <c r="F89" s="15" t="s">
+      <c r="F89" s="4" t="s">
         <v>117</v>
       </c>
       <c r="G89" s="4"/>
@@ -2953,7 +2955,7 @@
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
-      <c r="E113" s="15" t="s">
+      <c r="E113" s="4" t="s">
         <v>128</v>
       </c>
       <c r="F113" s="4"/>
@@ -3014,7 +3016,7 @@
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
-      <c r="F117" s="15" t="s">
+      <c r="F117" s="4" t="s">
         <v>132</v>
       </c>
       <c r="G117" s="4"/>
@@ -3247,7 +3249,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00ED00D2-00B9-44D5-820E-00A700CB0039}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0074005F-00AA-4018-9FFA-00CB00850090}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3264,7 +3266,7 @@
           <xm:sqref>I3:I112 I114:I126 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00720070-0016-435B-859D-006400120058}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00DC004E-00D4-42F0-B520-001B0076004A}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3281,7 +3283,7 @@
           <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E700EF-0089-4E2B-8B14-004500EF002C}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00C900C7-00CD-4D84-9CCC-0034006100F2}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3298,7 +3300,7 @@
           <xm:sqref>I127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00060092-0028-4FBD-BBCC-000100A40073}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00FE0060-008C-41AC-9938-00D90083009E}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3315,7 +3317,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{002C000F-0089-4660-AA7F-008600B80082}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00B00030-00DF-4AA5-9ED0-001100B00088}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3332,7 +3334,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00DA000F-004B-4CB4-B5CE-0072007500BF}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00090054-00E8-4F8D-88B5-00A600D0008D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3349,7 +3351,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{003800B1-008E-422F-BABC-009C006A0026}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00A9006C-009B-45E8-9D38-00A7005D00AE}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3366,7 +3368,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008D0007-0076-4399-9730-008900E900C4}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0020001E-0042-441E-A266-00E600E70093}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3383,7 +3385,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C80097-00AC-438F-BC78-00F7008A003F}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00760092-00F9-43FA-8278-007B00900003}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3400,7 +3402,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00FB00DB-00DC-4304-91C1-005500A6004C}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00A400F5-0032-452D-805E-003F0090006E}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3417,7 +3419,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00DA00C1-0038-49BC-A69F-004900DD0037}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{001800F7-0032-4FC9-BC3C-005200B10063}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3434,7 +3436,7 @@
           <xm:sqref>I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0040002C-00F3-4ECF-B58D-00290091005F}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0035004C-0093-46C7-87EC-009600D4001A}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3451,7 +3453,7 @@
           <xm:sqref>I131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00AB0072-00C7-412C-B661-0082006800B8}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D0002F-00C0-4A81-8B7A-0032006B00EB}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3468,7 +3470,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00BB00DC-0070-4013-80DF-009500CE0047}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B400DA-007C-4B38-B9A4-001000FD00D5}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3485,7 +3487,7 @@
           <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B70029-002F-4399-BF29-00D4007000A9}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001F000F-005B-4B8F-945E-005E00A600F8}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3502,7 +3504,7 @@
           <xm:sqref>I3:I112 I114:I126 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0007000B-0048-4528-B048-006A00C3008C}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00420092-0046-430E-8154-00110094001B}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3519,7 +3521,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00BB00A9-0085-47FD-BAA5-00B0007B0034}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C500AC-00FC-40A1-AE5D-005D008A0027}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3536,7 +3538,7 @@
           <xm:sqref>I127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0003001B-00B0-41A8-8E91-00B8001400F8}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{004100AA-008C-4D16-860E-003E006000AA}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3553,7 +3555,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B500F1-001C-4290-98C0-00C6004D00C2}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C4005C-00DC-4DA2-B427-00F300820055}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3570,7 +3572,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00CB00AC-001D-4E6C-84CA-00D200A70093}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00510097-0025-465D-BA22-007E006D007E}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3587,7 +3589,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00E20042-008B-44CB-8FA8-000800EA00FD}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{005D00B4-0074-4CC1-93AD-00250035009F}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3604,7 +3606,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00BC009F-0044-498D-AA3E-004800A100A6}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0054000E-002A-4A2F-AB24-00F4000100D5}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3621,7 +3623,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00BE001F-00A7-4D67-ABCC-00A7009900CC}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00110088-007D-4E6B-9E1F-0038008D0062}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3638,7 +3640,7 @@
           <xm:sqref>I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00720015-0019-4663-947A-00EB006600BB}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00690004-00F6-421B-91E2-000500A8002B}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3655,7 +3657,7 @@
           <xm:sqref>I131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00060048-0084-485D-9FD6-001300DE0059}">
+          <x14:cfRule type="dataBar" priority="2" id="{00A100ED-00F1-494B-97EE-00B200B4003B}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3671,7 +3673,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00CC0070-00D3-4D88-A74E-00CD009C009B}">
+          <x14:cfRule type="dataBar" priority="1" id="{00F300AE-0020-45EC-A26F-00580028003E}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
img msns complete; fixed msn list entry not deleting
</commit_message>
<xml_diff>
--- a/SatManager Work Breakdown Structure.xlsx
+++ b/SatManager Work Breakdown Structure.xlsx
@@ -384,16 +384,19 @@
     <t>lat/long</t>
   </si>
   <si>
-    <t xml:space="preserve">satellite imagery</t>
+    <t xml:space="preserve">display point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">experimental payload</t>
+  </si>
+  <si>
+    <t>de-orbit</t>
   </si>
   <si>
     <t xml:space="preserve">target satellite</t>
   </si>
   <si>
-    <t xml:space="preserve">experimental payload</t>
-  </si>
-  <si>
-    <t>de-orbit</t>
+    <t xml:space="preserve">show target</t>
   </si>
   <si>
     <t>rendevous</t>
@@ -409,9 +412,6 @@
   </si>
   <si>
     <t xml:space="preserve">select to view parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">highlight points when selected</t>
   </si>
   <si>
     <t xml:space="preserve">show reward</t>
@@ -462,32 +462,32 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.000000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <color rgb="FF006100"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.000000"/>
       <name val="Calibri"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -597,7 +597,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -636,9 +636,6 @@
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -669,7 +666,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J131" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J129" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1179,7 +1176,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A85" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1234,13 +1231,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.35384615384615387</v>
+        <v>0.4296875</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I126,"0")/ROWS(Table5[])</f>
-        <v>1.5384615384615385e-002</v>
+        <f>COUNTIF(I2:I124,"0")/ROWS(Table5[])</f>
+        <v>7.8125e-003</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1277,7 +1274,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1312,7 +1309,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -2234,7 +2231,7 @@
       <c r="I64" s="6">
         <v>1</v>
       </c>
-      <c r="J64" s="14" t="s">
+      <c r="J64" s="9" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2249,7 +2246,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="15">
+      <c r="I65" s="14">
         <v>1</v>
       </c>
       <c r="J65" s="9"/>
@@ -2533,7 +2530,9 @@
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
-      <c r="I84" s="6"/>
+      <c r="I84" s="6">
+        <v>0</v>
+      </c>
       <c r="J84" s="9"/>
     </row>
     <row r="85" ht="14.25">
@@ -2583,7 +2582,9 @@
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
-      <c r="I87" s="6"/>
+      <c r="I87" s="6">
+        <v>1</v>
+      </c>
       <c r="J87" s="9"/>
     </row>
     <row r="88" ht="14.25">
@@ -2645,7 +2646,9 @@
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
-      <c r="I91" s="6"/>
+      <c r="I91" s="6">
+        <v>1</v>
+      </c>
       <c r="J91" s="9"/>
     </row>
     <row r="92" ht="14.25">
@@ -2659,7 +2662,9 @@
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
-      <c r="I92" s="6"/>
+      <c r="I92" s="6">
+        <v>1</v>
+      </c>
       <c r="J92" s="9" t="s">
         <v>121</v>
       </c>
@@ -2687,7 +2692,7 @@
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
@@ -2703,11 +2708,13 @@
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
       <c r="F95" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
-      <c r="I95" s="6"/>
+      <c r="I95" s="6">
+        <v>1</v>
+      </c>
       <c r="J95" s="9"/>
     </row>
     <row r="96" ht="14.25">
@@ -2715,13 +2722,15 @@
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
-      <c r="E96" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
-      <c r="I96" s="6"/>
+      <c r="I96" s="6">
+        <v>1</v>
+      </c>
       <c r="J96" s="9"/>
     </row>
     <row r="97" ht="14.25">
@@ -2729,10 +2738,10 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4" t="s">
-        <v>124</v>
-      </c>
+      <c r="E97" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F97" s="4"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="6"/>
@@ -2745,7 +2754,7 @@
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
       <c r="F98" s="4" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
@@ -2759,7 +2768,7 @@
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
@@ -2771,10 +2780,10 @@
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
-      <c r="E100" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="6"/>
@@ -2785,10 +2794,10 @@
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
-      <c r="E101" s="4"/>
-      <c r="F101" s="4" t="s">
+      <c r="E101" s="11" t="s">
         <v>125</v>
       </c>
+      <c r="F101" s="4"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="6"/>
@@ -2801,7 +2810,7 @@
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
       <c r="F102" s="4" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
@@ -2815,7 +2824,7 @@
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
       <c r="F103" s="4" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
@@ -2827,10 +2836,10 @@
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
-      <c r="E104" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="F104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="6"/>
@@ -2843,7 +2852,7 @@
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
@@ -2851,60 +2860,60 @@
       <c r="J105" s="9"/>
     </row>
     <row r="106" ht="14.25">
-      <c r="A106" s="4"/>
-      <c r="B106" s="4"/>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
-      <c r="E106" s="4"/>
-      <c r="F106" s="4" t="s">
+      <c r="A106" s="11"/>
+      <c r="B106" s="11"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="11"/>
+      <c r="E106" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F106" s="11"/>
+      <c r="G106" s="11"/>
+      <c r="H106" s="11"/>
+      <c r="I106" s="13"/>
+      <c r="J106" s="10"/>
+    </row>
+    <row r="107" ht="14.25">
+      <c r="A107" s="11"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G107" s="11"/>
+      <c r="H107" s="11"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="10"/>
+    </row>
+    <row r="108" ht="14.25">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="9"/>
+    </row>
+    <row r="109" ht="14.25">
+      <c r="A109" s="4"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="G106" s="4"/>
-      <c r="H106" s="4"/>
-      <c r="I106" s="6"/>
-      <c r="J106" s="9"/>
-    </row>
-    <row r="107" ht="14.25">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
-      <c r="I107" s="6"/>
-      <c r="J107" s="9"/>
-    </row>
-    <row r="108" ht="14.25">
-      <c r="A108" s="11"/>
-      <c r="B108" s="11"/>
-      <c r="C108" s="11"/>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="F108" s="11"/>
-      <c r="G108" s="11"/>
-      <c r="H108" s="11"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="10"/>
-    </row>
-    <row r="109" ht="14.25">
-      <c r="A109" s="11"/>
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="G109" s="11"/>
-      <c r="H109" s="11"/>
-      <c r="I109" s="13"/>
-      <c r="J109" s="10"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="4"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="9"/>
     </row>
     <row r="110" ht="14.25">
       <c r="A110" s="4"/>
@@ -2913,7 +2922,7 @@
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
       <c r="F110" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
@@ -2924,29 +2933,31 @@
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
+      <c r="D111" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E111" s="4"/>
-      <c r="F111" s="4" t="s">
-        <v>119</v>
-      </c>
+      <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
-      <c r="I111" s="6"/>
+      <c r="I111" s="6">
+        <v>1</v>
+      </c>
       <c r="J111" s="9"/>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
-      <c r="D112" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J112" s="9"/>
     </row>
@@ -2956,12 +2967,14 @@
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="6"/>
+      <c r="I113" s="6">
+        <v>1</v>
+      </c>
       <c r="J113" s="9"/>
     </row>
     <row r="114" ht="14.25">
@@ -2969,14 +2982,14 @@
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
-      <c r="E114" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
       <c r="I114" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J114" s="9"/>
     </row>
@@ -2987,7 +3000,7 @@
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
@@ -3001,24 +3014,25 @@
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
-      <c r="E116" s="4"/>
       <c r="F116" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
-      <c r="I116" s="6"/>
+      <c r="I116" s="6">
+        <v>1</v>
+      </c>
       <c r="J116" s="9"/>
     </row>
     <row r="117" ht="14.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
+      <c r="D117" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="E117" s="4"/>
-      <c r="F117" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="6">
@@ -3031,22 +3045,25 @@
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
-      <c r="F118" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="E118" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118" s="4"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
-      <c r="I118" s="6"/>
+      <c r="I118" s="6">
+        <v>1</v>
+      </c>
       <c r="J118" s="9"/>
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
-      <c r="D119" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="E119" s="4"/>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
@@ -3058,42 +3075,38 @@
     <row r="120" ht="14.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
+      <c r="C120" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="D120" s="4"/>
-      <c r="E120" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E120" s="4"/>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
-      <c r="I120" s="6">
-        <v>1</v>
-      </c>
+      <c r="I120" s="6"/>
       <c r="J120" s="9"/>
     </row>
     <row r="121" ht="14.25">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
-      <c r="D121" s="4"/>
-      <c r="E121" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="D121" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E121" s="4"/>
       <c r="F121" s="4"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
-      <c r="I121" s="6">
-        <v>1</v>
-      </c>
+      <c r="I121" s="6"/>
       <c r="J121" s="9"/>
     </row>
     <row r="122" ht="14.25">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
-      <c r="C122" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
       <c r="G122" s="4"/>
@@ -3106,7 +3119,7 @@
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
@@ -3120,7 +3133,7 @@
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4" t="s">
-        <v>138</v>
+        <v>20</v>
       </c>
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
@@ -3131,11 +3144,11 @@
     </row>
     <row r="125" ht="14.25">
       <c r="A125" s="4"/>
-      <c r="B125" s="4"/>
+      <c r="B125" s="4" t="s">
+        <v>140</v>
+      </c>
       <c r="C125" s="4"/>
-      <c r="D125" s="4" t="s">
-        <v>139</v>
-      </c>
+      <c r="D125" s="4"/>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
       <c r="G125" s="4"/>
@@ -3146,91 +3159,65 @@
     <row r="126" ht="14.25">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
-      <c r="C126" s="4"/>
-      <c r="D126" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="C126" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D126" s="4"/>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
       <c r="I126" s="6"/>
-      <c r="J126" s="9"/>
+      <c r="J126" s="9" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="127" ht="14.25">
       <c r="A127" s="4"/>
-      <c r="B127" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C127" s="4"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
       <c r="G127" s="4"/>
       <c r="H127" s="4"/>
       <c r="I127" s="6"/>
-      <c r="J127" s="9"/>
+      <c r="J127" s="9" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="128" ht="14.25">
       <c r="A128" s="4"/>
-      <c r="B128" s="4"/>
-      <c r="C128" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="B128" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C128" s="4"/>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
       <c r="G128" s="4"/>
-      <c r="H128" s="4"/>
+      <c r="H128" s="15"/>
       <c r="I128" s="6"/>
-      <c r="J128" s="9" t="s">
-        <v>141</v>
-      </c>
+      <c r="J128" s="16"/>
     </row>
     <row r="129" ht="14.25">
-      <c r="A129" s="4"/>
-      <c r="B129" s="4"/>
-      <c r="C129" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D129" s="4"/>
-      <c r="E129" s="4"/>
-      <c r="F129" s="4"/>
-      <c r="G129" s="4"/>
-      <c r="H129" s="4"/>
+      <c r="C129" t="s">
+        <v>145</v>
+      </c>
       <c r="I129" s="6"/>
-      <c r="J129" s="9" t="s">
-        <v>143</v>
+      <c r="J129" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="130" ht="14.25">
-      <c r="A130" s="4"/>
-      <c r="B130" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C130" s="4"/>
-      <c r="D130" s="4"/>
-      <c r="E130" s="4"/>
-      <c r="F130" s="4"/>
-      <c r="G130" s="4"/>
-      <c r="H130" s="16"/>
-      <c r="I130" s="6"/>
+      <c r="C130" s="17"/>
+      <c r="I130" s="4"/>
       <c r="J130" s="17"/>
     </row>
-    <row r="131" ht="14.25">
-      <c r="C131" t="s">
-        <v>145</v>
-      </c>
-      <c r="I131" s="6"/>
-      <c r="J131" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="132" ht="14.25">
-      <c r="C132" s="18"/>
-      <c r="I132" s="4"/>
-      <c r="J132" s="18"/>
-    </row>
+    <row r="131" ht="14.25"/>
+    <row r="132" ht="14.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="L1:M1"/>
@@ -3240,7 +3227,7 @@
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483647" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3249,7 +3236,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0074005F-00AA-4018-9FFA-00CB00850090}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00730044-0030-4776-9FF7-008500B60064}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3263,10 +3250,163 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I112 I114:I126 I46:I49</xm:sqref>
+          <xm:sqref>I3:I111 I113:I124 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00DC004E-00D4-42F0-B520-001B0076004A}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D700A1-00F5-422F-9573-00D600630011}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I126</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00C000A2-00AF-4788-AF86-00B100FA00F8}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I125</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003F006E-00D2-4985-93AF-00C1006B00F2}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{006A007D-00B6-47DD-9830-00C5004C004E}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D7001B-0015-447E-A290-000F0057004C}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{002500EC-0090-4807-961A-000800E800A5}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00740062-002A-464C-925B-00AB00830001}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E80048-00CB-42D5-81A5-0006004C007F}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0029003B-00BE-455F-B793-00BC008E0031}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I66</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E6002B-0033-4E5A-9F7B-00860035009D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3283,7 +3423,7 @@
           <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C900C7-00CD-4D84-9CCC-0034006100F2}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004E00DF-00BE-4B69-BAFE-00AD0053003D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3297,10 +3437,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I127</xm:sqref>
+          <xm:sqref>I129</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00FE0060-008C-41AC-9938-00D90083009E}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0095006E-00D7-4BE5-B07C-0091009F0000}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3314,146 +3454,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I28</xm:sqref>
+          <xm:sqref>I112</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00B00030-00DF-4AA5-9ED0-001100B00088}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00090054-00E8-4F8D-88B5-00A600D0008D}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00A9006C-009B-45E8-9D38-00A7005D00AE}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I44</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0020001E-0042-441E-A266-00E600E70093}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I68</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00760092-00F9-43FA-8278-007B00900003}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I67</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00A400F5-0032-452D-805E-003F0090006E}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I66</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{001800F7-0032-4FC9-BC3C-005200B10063}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I130</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0035004C-0093-46C7-87EC-009600D4001A}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I131</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00D0002F-00C0-4A81-8B7A-0032006B00EB}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{007500C7-0058-455B-A9A0-002500F100C7}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3470,7 +3474,160 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B400DA-007C-4B38-B9A4-001000FD00D5}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00AA002A-0002-4809-81D2-007000C700E8}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I126</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{007500AD-00F8-4365-84C0-000E00C400AF}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I3:I111 I113:I124 I46:I49</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001A00B8-0042-4A96-BCDF-00AE002B00D8}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00620088-004B-48F9-91E3-009200680016}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I125</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001A00B0-0063-469D-B748-00110088008F}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00920093-003F-4CC7-AACC-001800BC005D}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001F00EB-0074-4A6F-82F3-00A400DA000F}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00990046-00FF-48C1-8D83-004A00DC0026}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00DE0084-00C0-4F9D-BE05-00B0005F0099}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I66</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{004D005A-00FA-4A17-AC4A-001100240051}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3487,7 +3644,7 @@
           <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{001F000F-005B-4B8F-945E-005E00A600F8}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{004B00D2-00D5-4AF8-A2E2-00BD009300AE}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3501,10 +3658,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I112 I114:I126 I46:I49</xm:sqref>
+          <xm:sqref>I129</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00420092-0046-430E-8154-00110094001B}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C200C9-00DD-413B-BDA6-009600330000}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3518,146 +3675,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I2</xm:sqref>
+          <xm:sqref>I112</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C500AC-00FC-40A1-AE5D-005D008A0027}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I127</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{004100AA-008C-4D16-860E-003E006000AA}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C4005C-00DC-4DA2-B427-00F300820055}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I44</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00510097-0025-465D-BA22-007E006D007E}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I68</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{005D00B4-0074-4CC1-93AD-00250035009F}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I67</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0054000E-002A-4A2F-AB24-00F4000100D5}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I66</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00110088-007D-4E6B-9E1F-0038008D0062}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I130</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00690004-00F6-421B-91E2-000500A8002B}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I131</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00A100ED-00F1-494B-97EE-00B200B4003B}">
+          <x14:cfRule type="dataBar" priority="2" id="{009D006F-0080-4C91-9830-00940033000E}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3673,7 +3694,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00F300AE-0020-45EC-A26F-00580028003E}">
+          <x14:cfRule type="dataBar" priority="1" id="{004D00CA-0093-41DE-8C5F-004200E50093}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
draft code for exp & grapple mission details
</commit_message>
<xml_diff>
--- a/SatManager Work Breakdown Structure.xlsx
+++ b/SatManager Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="151">
   <si>
     <t>Status</t>
   </si>
@@ -126,7 +126,7 @@
     <t>fuel</t>
   </si>
   <si>
-    <t xml:space="preserve">measure fuel in deltaV. deltaV = exhaust exit speed -&gt; total propelant mass of 1.7 x vehicle dry mass</t>
+    <t xml:space="preserve">measure fuel in deltaV</t>
   </si>
   <si>
     <t>ui</t>
@@ -454,6 +454,18 @@
   </si>
   <si>
     <t xml:space="preserve">reduce the number of GetComponent calls as much as possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fine Tuning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuel amounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimum viewing angles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">experiment altitude parameters</t>
   </si>
 </sst>
 </file>
@@ -597,7 +609,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -621,6 +633,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="4" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -666,7 +681,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J129" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J134" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1176,7 +1191,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A113" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1231,13 +1246,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.4296875</v>
+        <v>0.41353383458646614</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f>COUNTIF(I2:I124,"0")/ROWS(Table5[])</f>
-        <v>7.8125e-003</v>
+        <v>7.5187969924812026e-003</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1274,7 +1289,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1726,7 +1741,7 @@
       <c r="I34" s="6">
         <v>1</v>
       </c>
-      <c r="J34" s="10" t="s">
+      <c r="J34" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1828,7 +1843,7 @@
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E41" s="4"/>
@@ -1844,7 +1859,7 @@
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="12" t="s">
         <v>52</v>
       </c>
       <c r="F42" s="4"/>
@@ -1866,26 +1881,26 @@
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
-      <c r="I43" s="12">
+      <c r="I43" s="13">
         <v>1</v>
       </c>
       <c r="J43" s="9"/>
     </row>
     <row r="44" ht="28.5">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11" t="s">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="13">
-        <v>1</v>
-      </c>
-      <c r="J44" s="10" t="s">
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="14">
+        <v>1</v>
+      </c>
+      <c r="J44" s="11" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1974,20 +1989,20 @@
       </c>
     </row>
     <row r="50" ht="28.5">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11" t="s">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="13">
-        <v>1</v>
-      </c>
-      <c r="J50" s="10" t="s">
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="14">
+        <v>1</v>
+      </c>
+      <c r="J50" s="11" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2246,7 +2261,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="14">
+      <c r="I65" s="15">
         <v>1</v>
       </c>
       <c r="J65" s="9"/>
@@ -2406,18 +2421,18 @@
       <c r="J75" s="9"/>
     </row>
     <row r="76" ht="28.5">
-      <c r="A76" s="11"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11" t="s">
+      <c r="A76" s="12"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="10" t="s">
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="11" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2794,7 +2809,7 @@
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
-      <c r="E101" s="11" t="s">
+      <c r="E101" s="12" t="s">
         <v>125</v>
       </c>
       <c r="F101" s="4"/>
@@ -2860,32 +2875,32 @@
       <c r="J105" s="9"/>
     </row>
     <row r="106" ht="14.25">
-      <c r="A106" s="11"/>
-      <c r="B106" s="11"/>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11" t="s">
+      <c r="A106" s="12"/>
+      <c r="B106" s="12"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="F106" s="11"/>
-      <c r="G106" s="11"/>
-      <c r="H106" s="11"/>
-      <c r="I106" s="13"/>
-      <c r="J106" s="10"/>
+      <c r="F106" s="12"/>
+      <c r="G106" s="12"/>
+      <c r="H106" s="12"/>
+      <c r="I106" s="14"/>
+      <c r="J106" s="11"/>
     </row>
     <row r="107" ht="14.25">
-      <c r="A107" s="11"/>
-      <c r="B107" s="11"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11" t="s">
+      <c r="A107" s="12"/>
+      <c r="B107" s="12"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="G107" s="11"/>
-      <c r="H107" s="11"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="10"/>
+      <c r="G107" s="12"/>
+      <c r="H107" s="12"/>
+      <c r="I107" s="14"/>
+      <c r="J107" s="11"/>
     </row>
     <row r="108" ht="14.25">
       <c r="A108" s="4"/>
@@ -3198,9 +3213,9 @@
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
       <c r="G128" s="4"/>
-      <c r="H128" s="15"/>
+      <c r="H128" s="16"/>
       <c r="I128" s="6"/>
-      <c r="J128" s="16"/>
+      <c r="J128" s="17"/>
     </row>
     <row r="129" ht="14.25">
       <c r="C129" t="s">
@@ -3212,12 +3227,33 @@
       </c>
     </row>
     <row r="130" ht="14.25">
-      <c r="C130" s="17"/>
+      <c r="B130" t="s">
+        <v>147</v>
+      </c>
+      <c r="C130" s="18"/>
       <c r="I130" s="4"/>
-      <c r="J130" s="17"/>
-    </row>
-    <row r="131" ht="14.25"/>
-    <row r="132" ht="14.25"/>
+      <c r="J130" s="18"/>
+    </row>
+    <row r="131" ht="14.25">
+      <c r="C131" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="132" ht="14.25">
+      <c r="C132" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="133" ht="14.25">
+      <c r="C133" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="134" ht="14.25">
+      <c r="C134" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="L1:M1"/>
@@ -3236,7 +3272,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00730044-0030-4776-9FF7-008500B60064}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00B7002F-004F-4AFC-BFCF-007F00F30029}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3253,7 +3289,7 @@
           <xm:sqref>I3:I111 I113:I124 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D700A1-00F5-422F-9573-00D600630011}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{008F003D-00CA-4E29-A023-005000C20096}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3270,7 +3306,7 @@
           <xm:sqref>I126</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C000A2-00AF-4788-AF86-00B100FA00F8}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00F100B8-00ED-44D9-920D-002000F3008A}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3287,7 +3323,7 @@
           <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{003F006E-00D2-4985-93AF-00C1006B00F2}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00A10036-0005-41C9-BECE-005A00E10064}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3304,7 +3340,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{006A007D-00B6-47DD-9830-00C5004C004E}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004500FF-0027-46C7-854C-00DC006F005B}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3321,7 +3357,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D7001B-0015-447E-A290-000F0057004C}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E9008D-00A7-4537-848F-0078007F00F8}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3338,7 +3374,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{002500EC-0090-4807-961A-000800E800A5}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007E0013-00A1-4E90-B646-0074007C0097}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3355,7 +3391,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00740062-002A-464C-925B-00AB00830001}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005600F3-0073-44DC-9943-000A00D100EA}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3372,7 +3408,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E80048-00CB-42D5-81A5-0006004C007F}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00AA0046-0041-4B3C-ABFA-00E8006F0076}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3389,7 +3425,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0029003B-00BE-455F-B793-00BC008E0031}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00140059-0070-4662-B708-00B1004C0014}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3406,7 +3442,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E6002B-0033-4E5A-9F7B-00860035009D}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0015002A-002B-4D15-A7A6-007B00DE0071}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3423,7 +3459,7 @@
           <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{004E00DF-00BE-4B69-BAFE-00AD0053003D}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{009000EF-00E2-48B0-BA38-004F00A4008E}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3440,7 +3476,7 @@
           <xm:sqref>I129</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0095006E-00D7-4BE5-B07C-0091009F0000}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004D008F-00C6-45A3-B4C5-00AC009E0041}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3457,7 +3493,7 @@
           <xm:sqref>I112</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{007500C7-0058-455B-A9A0-002500F100C7}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00780026-004E-43F0-B174-000400CF00B2}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3474,7 +3510,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00AA002A-0002-4809-81D2-007000C700E8}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00200085-00B4-47AF-B914-003D00C200E0}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3491,7 +3527,7 @@
           <xm:sqref>I126</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{007500AD-00F8-4365-84C0-000E00C400AF}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B800B0-0079-498B-AD96-003200030019}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3508,7 +3544,7 @@
           <xm:sqref>I3:I111 I113:I124 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{001A00B8-0042-4A96-BCDF-00AE002B00D8}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0098005F-00DD-4743-848F-002F00A10085}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3525,7 +3561,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00620088-004B-48F9-91E3-009200680016}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{007D007E-0068-442A-91BB-007800B3009C}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3542,7 +3578,7 @@
           <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{001A00B0-0063-469D-B748-00110088008F}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000500AD-0064-49A7-A177-00C300D000AB}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3559,7 +3595,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00920093-003F-4CC7-AACC-001800BC005D}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003400C0-0060-47B6-A342-00B900950054}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3576,7 +3612,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{001F00EB-0074-4A6F-82F3-00A400DA000F}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00F20040-00AF-4565-A446-007A0023000A}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3593,7 +3629,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00990046-00FF-48C1-8D83-004A00DC0026}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{008B00E8-00E7-4158-99C7-0016009E0099}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3610,7 +3646,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00DE0084-00C0-4F9D-BE05-00B0005F0099}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{002E0029-0062-4245-BBB8-001400AF009C}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3627,7 +3663,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{004D005A-00FA-4A17-AC4A-001100240051}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{006E00A7-00C0-4779-AF28-00EE00030004}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3644,7 +3680,7 @@
           <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{004B00D2-00D5-4AF8-A2E2-00BD009300AE}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C300B9-0063-4951-80CD-009300CA0098}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3661,7 +3697,7 @@
           <xm:sqref>I129</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C200C9-00DD-413B-BDA6-009600330000}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000A00ED-00F2-49C2-AF80-00E500390070}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3678,7 +3714,7 @@
           <xm:sqref>I112</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{009D006F-0080-4C91-9830-00940033000E}">
+          <x14:cfRule type="dataBar" priority="2" id="{00010081-00D7-44D1-86C0-003800080079}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3694,7 +3730,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{004D00CA-0093-41DE-8C5F-004200E50093}">
+          <x14:cfRule type="dataBar" priority="1" id="{00CC00EB-00C1-411B-892D-00D900F400F4}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
modified new sat func; progress on grappling
new sat function now takes bool that controls if the satellite should be added to the list.
new satellite type "target" gets added to mission system bucket.
</commit_message>
<xml_diff>
--- a/SatManager Work Breakdown Structure.xlsx
+++ b/SatManager Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>Status</t>
   </si>
@@ -180,7 +180,7 @@
     <t xml:space="preserve">display position</t>
   </si>
   <si>
-    <t xml:space="preserve">highlight current position, trail length based on game speed</t>
+    <t xml:space="preserve">current position w/ sphere, trail length based on game speed</t>
   </si>
   <si>
     <t xml:space="preserve">satellite management</t>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>attach/detach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set object references, set position to match grappler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en/dis orbital mechanics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set all parameters to match grabbler</t>
   </si>
   <si>
     <t>maneuver</t>
@@ -591,7 +600,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -630,6 +639,12 @@
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -660,7 +675,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J127" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J129" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1170,15 +1185,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A110" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A84" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="6" width="2.7109375"/>
-    <col bestFit="1" min="7" max="7" width="11.00390625"/>
-    <col customWidth="1" min="8" max="8" width="12.57421875"/>
+    <col customWidth="1" min="1" max="7" width="2.7109375"/>
+    <col customWidth="1" min="8" max="8" width="21.7109375"/>
     <col customWidth="1" min="10" max="10" width="45.7109375"/>
     <col bestFit="1" customWidth="1" min="11" max="11" width="9.140625"/>
     <col bestFit="1" customWidth="1" min="14" max="14" width="9.140625"/>
@@ -1225,13 +1239,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.42857142857142855</v>
+        <v>0.4140625</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I118,"0")/ROWS(Table5[])</f>
-        <v>7.9365079365079361e-003</v>
+        <f>COUNTIF(I2:I120,"0")/ROWS(Table5[])</f>
+        <v>3.90625e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1268,7 +1282,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1303,7 +1317,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1876,10 +1890,8 @@
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
-      <c r="I44" s="13">
-        <v>1</v>
-      </c>
-      <c r="J44" s="10" t="s">
+      <c r="I44" s="13"/>
+      <c r="J44" s="14" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2067,25 +2079,25 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="6"/>
-      <c r="J55" s="9" t="s">
-        <v>75</v>
-      </c>
+      <c r="J55" s="9"/>
     </row>
     <row r="56" ht="14.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
+      <c r="G56" s="15" t="s">
+        <v>75</v>
+      </c>
       <c r="H56" s="4"/>
       <c r="I56" s="6">
-        <v>1</v>
-      </c>
-      <c r="J56" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="14" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="57" ht="14.25">
       <c r="A57" s="4"/>
@@ -2093,16 +2105,16 @@
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
-      <c r="F57" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="15" t="s">
+        <v>77</v>
+      </c>
       <c r="H57" s="4"/>
       <c r="I57" s="6">
-        <v>1</v>
-      </c>
-      <c r="J57" s="9" t="s">
-        <v>77</v>
+        <v>0</v>
+      </c>
+      <c r="J57" s="14" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="58" ht="14.25">
@@ -2110,18 +2122,16 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="E58" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="6">
         <v>1</v>
       </c>
-      <c r="J58" s="9" t="s">
-        <v>79</v>
-      </c>
+      <c r="J58" s="9"/>
     </row>
     <row r="59" ht="28.5">
       <c r="A59" s="4"/>
@@ -2130,7 +2140,7 @@
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="F59" s="4" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
@@ -2138,7 +2148,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" ht="28.5">
@@ -2146,17 +2156,17 @@
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
-      <c r="E60" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="6">
         <v>1</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" ht="28.5">
@@ -2164,17 +2174,17 @@
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
-      <c r="E61" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="6">
         <v>1</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" ht="14.25">
@@ -2183,7 +2193,7 @@
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -2192,53 +2202,57 @@
         <v>1</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" ht="14.25">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
-      <c r="D63" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
-      <c r="I63" s="14">
-        <v>1</v>
-      </c>
-      <c r="J63" s="9"/>
+      <c r="I63" s="6">
+        <v>1</v>
+      </c>
+      <c r="J63" s="9" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="64" ht="28.5">
       <c r="A64" s="4"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="4"/>
+      <c r="E64" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="6">
         <v>1</v>
       </c>
-      <c r="J64" s="9"/>
+      <c r="J64" s="9" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="65" ht="14.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="D65" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="6">
+      <c r="I65" s="16">
         <v>1</v>
       </c>
       <c r="J65" s="9"/>
@@ -2247,10 +2261,10 @@
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="D66" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
@@ -2262,11 +2276,11 @@
     <row r="67" ht="14.25">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
-      <c r="C67" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="C67" s="4"/>
       <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
+      <c r="E67" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
@@ -2279,49 +2293,51 @@
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
-      <c r="D68" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="6">
         <v>1</v>
       </c>
-      <c r="J68" s="9" t="s">
-        <v>94</v>
-      </c>
+      <c r="J68" s="9"/>
     </row>
     <row r="69" ht="14.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="D69" s="4"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="9" t="s">
-        <v>96</v>
-      </c>
+      <c r="I69" s="6">
+        <v>1</v>
+      </c>
+      <c r="J69" s="9"/>
     </row>
     <row r="70" ht="14.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
-      <c r="I70" s="6"/>
-      <c r="J70" s="9"/>
+      <c r="I70" s="6">
+        <v>1</v>
+      </c>
+      <c r="J70" s="9" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="71" ht="14.25">
       <c r="A71" s="4"/>
@@ -2335,16 +2351,18 @@
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="6"/>
-      <c r="J71" s="9"/>
+      <c r="J71" s="9" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
+      <c r="C72" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="D72" s="4"/>
-      <c r="E72" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
@@ -2355,10 +2373,10 @@
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="D73" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
@@ -2366,29 +2384,27 @@
       <c r="J73" s="9"/>
     </row>
     <row r="74" ht="14.25">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="10" t="s">
-        <v>101</v>
-      </c>
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="9"/>
     </row>
     <row r="75" ht="14.25">
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="4"/>
+      <c r="E75" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
@@ -2396,27 +2412,29 @@
       <c r="J75" s="9"/>
     </row>
     <row r="76" ht="28.5">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4" t="s">
+      <c r="A76" s="11"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="6"/>
-      <c r="J76" s="9"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="10" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="77" ht="28.5">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4" t="s">
-        <v>104</v>
-      </c>
+      <c r="D77" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E77" s="4"/>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
@@ -2429,7 +2447,7 @@
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
@@ -2441,10 +2459,10 @@
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
-      <c r="D79" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
@@ -2457,7 +2475,7 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -2469,10 +2487,10 @@
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4" t="s">
-        <v>106</v>
-      </c>
+      <c r="D81" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E81" s="4"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
@@ -2482,96 +2500,92 @@
     <row r="82" ht="14.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
-      <c r="C82" s="4" t="s">
-        <v>107</v>
-      </c>
+      <c r="C82" s="4"/>
       <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
+      <c r="E82" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
-      <c r="I82" s="6">
-        <v>0</v>
-      </c>
+      <c r="I82" s="6"/>
       <c r="J82" s="9"/>
     </row>
     <row r="83" ht="14.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
-      <c r="D83" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
-      <c r="I83" s="6">
-        <v>1</v>
-      </c>
-      <c r="J83" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="I83" s="6"/>
+      <c r="J83" s="9"/>
     </row>
     <row r="84" ht="14.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="D84" s="4"/>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="6">
-        <v>1</v>
-      </c>
-      <c r="J84" s="9" t="s">
-        <v>111</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J84" s="9"/>
     </row>
     <row r="85" ht="14.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4" t="s">
-        <v>68</v>
-      </c>
+      <c r="D85" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
       <c r="I85" s="6">
         <v>1</v>
       </c>
-      <c r="J85" s="9"/>
+      <c r="J85" s="9" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="86" ht="14.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
+      <c r="D86" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="E86" s="4"/>
-      <c r="F86" s="4" t="s">
-        <v>112</v>
-      </c>
+      <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="6">
         <v>1</v>
       </c>
-      <c r="J86" s="9"/>
+      <c r="J86" s="9" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="87" ht="14.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="4" t="s">
-        <v>113</v>
-      </c>
+      <c r="E87" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="6">
@@ -2586,7 +2600,7 @@
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
       <c r="F88" s="4" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
@@ -2602,7 +2616,7 @@
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
@@ -2616,18 +2630,16 @@
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
-      <c r="E90" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="6">
         <v>1</v>
       </c>
-      <c r="J90" s="9" t="s">
-        <v>117</v>
-      </c>
+      <c r="J90" s="9"/>
     </row>
     <row r="91" ht="14.25">
       <c r="A91" s="4"/>
@@ -2650,16 +2662,18 @@
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4" t="s">
+      <c r="E92" s="4" t="s">
         <v>119</v>
       </c>
+      <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="6">
         <v>1</v>
       </c>
-      <c r="J92" s="9"/>
+      <c r="J92" s="9" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="93" ht="14.25">
       <c r="A93" s="4"/>
@@ -2668,7 +2682,7 @@
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -2684,7 +2698,7 @@
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
@@ -2698,13 +2712,15 @@
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
-      <c r="E95" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F95" s="4"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
-      <c r="I95" s="6"/>
+      <c r="I95" s="6">
+        <v>1</v>
+      </c>
       <c r="J95" s="9"/>
     </row>
     <row r="96" ht="14.25">
@@ -2714,11 +2730,13 @@
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
-      <c r="I96" s="6"/>
+      <c r="I96" s="6">
+        <v>1</v>
+      </c>
       <c r="J96" s="9"/>
     </row>
     <row r="97" ht="14.25">
@@ -2726,10 +2744,10 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4" t="s">
-        <v>122</v>
-      </c>
+      <c r="E97" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F97" s="4"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="6"/>
@@ -2742,11 +2760,13 @@
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
       <c r="F98" s="4" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
-      <c r="I98" s="6"/>
+      <c r="I98" s="6">
+        <v>0</v>
+      </c>
       <c r="J98" s="9"/>
     </row>
     <row r="99" ht="14.25">
@@ -2756,7 +2776,7 @@
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
@@ -2764,60 +2784,62 @@
       <c r="J99" s="9"/>
     </row>
     <row r="100" ht="14.25">
-      <c r="A100" s="11"/>
-      <c r="B100" s="11"/>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="10"/>
+      <c r="A100" s="4"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="4"/>
+      <c r="E100" s="4"/>
+      <c r="F100" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G100" s="4"/>
+      <c r="H100" s="4"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="9"/>
     </row>
     <row r="101" ht="14.25">
-      <c r="A101" s="11"/>
-      <c r="B101" s="11"/>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
-      <c r="F101" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="10"/>
+      <c r="A101" s="4"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="9"/>
     </row>
     <row r="102" ht="14.25">
-      <c r="A102" s="4"/>
-      <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
-      <c r="E102" s="4"/>
-      <c r="F102" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G102" s="4"/>
-      <c r="H102" s="4"/>
-      <c r="I102" s="6"/>
-      <c r="J102" s="9"/>
+      <c r="A102" s="11"/>
+      <c r="B102" s="11"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="11"/>
+      <c r="E102" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F102" s="11"/>
+      <c r="G102" s="11"/>
+      <c r="H102" s="11"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="10"/>
     </row>
     <row r="103" ht="14.25">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="6"/>
-      <c r="J103" s="9"/>
+      <c r="A103" s="11"/>
+      <c r="B103" s="11"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G103" s="11"/>
+      <c r="H103" s="11"/>
+      <c r="I103" s="13">
+        <v>0</v>
+      </c>
+      <c r="J103" s="10"/>
     </row>
     <row r="104" ht="14.25">
       <c r="A104" s="4"/>
@@ -2826,7 +2848,7 @@
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
       <c r="F104" s="4" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
@@ -2837,16 +2859,14 @@
       <c r="A105" s="4"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
-      <c r="D105" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D105" s="4"/>
       <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
+      <c r="F105" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
-      <c r="I105" s="6">
-        <v>1</v>
-      </c>
+      <c r="I105" s="6"/>
       <c r="J105" s="9"/>
     </row>
     <row r="106" ht="14.25">
@@ -2854,25 +2874,23 @@
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
-      <c r="E106" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F106" s="4"/>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
-      <c r="I106" s="6">
-        <v>1</v>
-      </c>
+      <c r="I106" s="6"/>
       <c r="J106" s="9"/>
     </row>
     <row r="107" ht="14.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4" t="s">
-        <v>125</v>
-      </c>
+      <c r="D107" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" s="4"/>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
@@ -2886,10 +2904,10 @@
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
-      <c r="E108" s="4"/>
-      <c r="F108" s="4" t="s">
-        <v>126</v>
-      </c>
+      <c r="E108" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="6">
@@ -2902,10 +2920,10 @@
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
-      <c r="E109" s="4"/>
-      <c r="F109" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="E109" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="6">
@@ -2918,8 +2936,9 @@
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
+      <c r="E110" s="4"/>
       <c r="F110" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
@@ -2932,11 +2951,11 @@
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
-      <c r="D111" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="D111" s="4"/>
       <c r="E111" s="4"/>
-      <c r="F111" s="4"/>
+      <c r="F111" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
       <c r="I111" s="6">
@@ -2949,10 +2968,9 @@
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
-      <c r="E112" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F112" s="4"/>
+      <c r="F112" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="6">
@@ -2964,10 +2982,10 @@
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
-      <c r="D113" s="4"/>
-      <c r="E113" s="4" t="s">
-        <v>130</v>
-      </c>
+      <c r="D113" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E113" s="4"/>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
@@ -2979,38 +2997,42 @@
     <row r="114" ht="14.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
-      <c r="C114" s="4" t="s">
-        <v>131</v>
-      </c>
+      <c r="C114" s="4"/>
       <c r="D114" s="4"/>
-      <c r="E114" s="4"/>
+      <c r="E114" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
-      <c r="I114" s="6"/>
+      <c r="I114" s="6">
+        <v>1</v>
+      </c>
       <c r="J114" s="9"/>
     </row>
     <row r="115" ht="14.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
-      <c r="D115" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
-      <c r="I115" s="6"/>
+      <c r="I115" s="6">
+        <v>1</v>
+      </c>
       <c r="J115" s="9"/>
     </row>
     <row r="116" ht="14.25">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
-      <c r="C116" s="4"/>
-      <c r="D116" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="C116" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D116" s="4"/>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
       <c r="G116" s="4"/>
@@ -3023,7 +3045,7 @@
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
@@ -3037,7 +3059,7 @@
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
@@ -3048,11 +3070,11 @@
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
-      <c r="B119" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="B119" s="4"/>
       <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
+      <c r="D119" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
@@ -3063,86 +3085,112 @@
     <row r="120" ht="14.25">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
-      <c r="C120" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="E120" s="4"/>
       <c r="F120" s="4"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
       <c r="I120" s="6"/>
-      <c r="J120" s="9" t="s">
-        <v>136</v>
-      </c>
+      <c r="J120" s="9"/>
     </row>
     <row r="121" ht="14.25">
       <c r="A121" s="4"/>
-      <c r="B121" s="4"/>
-      <c r="C121" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="B121" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
       <c r="I121" s="6"/>
-      <c r="J121" s="9" t="s">
-        <v>138</v>
-      </c>
+      <c r="J121" s="9"/>
     </row>
     <row r="122" ht="14.25">
       <c r="A122" s="4"/>
-      <c r="B122" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C122" s="4"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
       <c r="G122" s="4"/>
-      <c r="H122" s="15"/>
+      <c r="H122" s="4"/>
       <c r="I122" s="6"/>
-      <c r="J122" s="16"/>
+      <c r="J122" s="9" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="123" ht="14.25">
-      <c r="C123" t="s">
+      <c r="A123" s="4"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="4" t="s">
         <v>140</v>
       </c>
+      <c r="D123" s="4"/>
+      <c r="E123" s="4"/>
+      <c r="F123" s="4"/>
+      <c r="G123" s="4"/>
+      <c r="H123" s="4"/>
       <c r="I123" s="6"/>
-      <c r="J123" t="s">
+      <c r="J123" s="9" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="124" ht="14.25">
-      <c r="B124" t="s">
+      <c r="A124" s="4"/>
+      <c r="B124" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C124" s="17"/>
+      <c r="C124" s="4"/>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4"/>
+      <c r="F124" s="4"/>
+      <c r="G124" s="4"/>
+      <c r="H124" s="17"/>
       <c r="I124" s="6"/>
-      <c r="J124" s="17"/>
-    </row>
-    <row r="125" ht="14.25">
+      <c r="J124" s="18"/>
+    </row>
+    <row r="125" ht="28.5">
       <c r="C125" t="s">
         <v>143</v>
       </c>
       <c r="I125" s="6"/>
+      <c r="J125" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="126" ht="14.25">
-      <c r="C126" t="s">
-        <v>144</v>
-      </c>
+      <c r="B126" t="s">
+        <v>145</v>
+      </c>
+      <c r="C126" s="19"/>
       <c r="I126" s="6"/>
+      <c r="J126" s="19"/>
     </row>
     <row r="127" ht="14.25">
       <c r="C127" t="s">
-        <v>91</v>
+        <v>146</v>
       </c>
       <c r="I127" s="6"/>
     </row>
-    <row r="128" ht="14.25"/>
-    <row r="129" ht="14.25"/>
+    <row r="128" ht="14.25">
+      <c r="C128" t="s">
+        <v>147</v>
+      </c>
+      <c r="I128" s="6"/>
+    </row>
+    <row r="129" ht="14.25">
+      <c r="C129" t="s">
+        <v>94</v>
+      </c>
+      <c r="I129" s="6"/>
+    </row>
     <row r="130" ht="14.25"/>
     <row r="131" ht="14.25"/>
     <row r="132" ht="14.25"/>
@@ -3166,7 +3214,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{002C0052-00B0-4B6F-890B-00810054004A}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{008D00AC-00F0-4533-A424-001A00C800AC}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3180,10 +3228,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I105 I107:I118 I46:I49</xm:sqref>
+          <xm:sqref>I3:I107 I109:I120 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C30023-00CD-41C4-B16C-007F0004008E}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00B00071-0006-4F72-AD5B-0052008E00DB}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3197,10 +3245,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I120</xm:sqref>
+          <xm:sqref>I122</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0055000D-0068-48A7-A699-00390091002A}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D700E0-00A9-4879-B4E1-0006003200A1}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3214,10 +3262,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I119</xm:sqref>
+          <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00FE0030-004C-4B52-BE54-00F000BB0008}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00BA0092-00D2-47CA-B9B6-000D0041004F}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3234,7 +3282,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00EC0053-00B7-4A87-B733-004700760056}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E80081-00AD-4C2B-B86B-005F003D003A}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3251,7 +3299,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E2005F-00DA-430A-B11F-00C6006B0009}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0041008E-001B-4A28-9BA8-009A001D003B}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3268,7 +3316,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00B800E2-005D-4424-B5D5-005900750055}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007B00FD-002E-4A8F-BCA7-008000CB002D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3285,7 +3333,41 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00DA008D-00D9-4622-9164-00CE00250036}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{009E00F4-00B0-48F2-B3BA-007600A40073}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{008800FF-009D-4228-B8C3-000700FC006F}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{006A008F-00A4-42CD-93B9-005F0097000C}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3302,92 +3384,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C500B6-005C-40D4-BAB5-005A003F00EB}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I65</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008D00D7-00E9-420F-8BFE-0015003A0076}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I64</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0059000D-00F5-442C-8B4D-007900C4001D}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I122</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E5009A-00EC-4486-8302-00E7003C00EC}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I123</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00000063-00A9-4A00-AA55-002300360030}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I106</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{000C0073-0001-4B7C-9DCF-00D300FA00FD}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00480076-00AA-45BD-9D25-00D100310035}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3404,7 +3401,58 @@
           <xm:sqref>I124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00800076-0039-4665-A7C9-0003000500AA}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007D006D-0047-429D-8EA9-005200F7005C}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I125</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0035008F-0046-4C52-A378-00FB000C00F4}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I108</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00F100DB-0029-4F88-88D8-008B000500F7}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I126</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000600B5-00A4-412C-9EA3-00E3006D0061}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3421,7 +3469,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0069003F-008B-4526-98F9-00A400860050}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001E0066-001D-4CF2-87CA-0088004200B2}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3435,10 +3483,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I120</xm:sqref>
+          <xm:sqref>I122</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00E40042-00A6-45B0-B0E0-000800E3004E}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B60097-0032-43D0-8AD0-002400750070}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3452,10 +3500,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I105 I107:I118 I46:I49</xm:sqref>
+          <xm:sqref>I3:I107 I109:I120 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00A6001B-002B-4FF8-965B-0067003200C8}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{009E00DA-0033-4A81-824C-0005006E00A3}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3472,7 +3520,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00750005-0030-4C77-A013-005E00C00023}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{007D0021-00A4-4803-9D69-009C00860058}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3486,10 +3534,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I119</xm:sqref>
+          <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00AC0064-00C1-4AA9-AD0D-006B008D008A}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{004A0045-00BC-441A-B065-0000008B001F}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3506,7 +3554,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00BB003C-005A-478E-8D1C-007200CE006D}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D40081-00E9-45CB-9516-00690040008C}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3523,7 +3571,41 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00A400B7-006E-442C-B969-003B006A00FC}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003B00F4-0049-41E1-9B60-00B500DA00BA}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00740022-0032-496B-89BE-00E6008400C3}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C90073-00AC-483C-ADC2-00A200DC0049}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3540,92 +3622,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{007F00A3-00E3-4C0B-9CF2-00F2007E00B0}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I65</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F700F1-0093-4BB8-AD09-00A500D900C3}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I64</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00CB0037-00CD-4742-91D0-00CA008000B3}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I122</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{004E002F-00D2-40C0-9EC4-00B6002B00C4}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I123</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00E80036-0058-4EC9-9B2F-002700C5007B}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I106</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{009200CE-000B-42FA-9AB3-00BB00F00023}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{005700B3-00F1-436A-BC8E-00B1007400F0}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3642,7 +3639,58 @@
           <xm:sqref>I124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{005E001C-0007-4074-A5C6-00760080004B}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{008E0091-00F4-47D0-8359-0083005200E1}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I125</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B50020-00D7-488C-A7ED-00A800700049}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I108</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00630059-0073-4D81-B929-0056003C00D8}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I126</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" priority="2" id="{00070097-00D4-41D6-8F82-00E600190043}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3658,7 +3706,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00EC006B-005F-425B-B230-004000FB0046}">
+          <x14:cfRule type="dataBar" priority="1" id="{00610019-00BB-4275-BD7E-005700DC00C2}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
added grapple target satellites
</commit_message>
<xml_diff>
--- a/SatManager Work Breakdown Structure.xlsx
+++ b/SatManager Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>Status</t>
   </si>
@@ -384,16 +384,13 @@
     <t xml:space="preserve">display point</t>
   </si>
   <si>
-    <t>de-orbit</t>
+    <t>grapple</t>
   </si>
   <si>
     <t xml:space="preserve">target satellite</t>
   </si>
   <si>
     <t xml:space="preserve">show target</t>
-  </si>
-  <si>
-    <t>rendevous</t>
   </si>
   <si>
     <t xml:space="preserve">selected mission details</t>
@@ -639,14 +636,14 @@
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -675,7 +672,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J129" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J124" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1185,7 +1182,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A84" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A79" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1239,13 +1236,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.4140625</v>
+        <v>0.43902439024390244</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I120,"0")/ROWS(Table5[])</f>
-        <v>3.90625e-002</v>
+        <f>COUNTIF(I2:I115,"0")/ROWS(Table5[])</f>
+        <v>2.4390243902439025e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1282,7 +1279,7 @@
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1317,7 +1314,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1891,7 +1888,7 @@
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="13"/>
-      <c r="J44" s="14" t="s">
+      <c r="J44" s="9" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2088,14 +2085,14 @@
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="15" t="s">
+      <c r="G56" s="4" t="s">
         <v>75</v>
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="6">
         <v>0</v>
       </c>
-      <c r="J56" s="14" t="s">
+      <c r="J56" s="9" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2106,14 +2103,14 @@
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="15" t="s">
+      <c r="G57" s="4" t="s">
         <v>77</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="6">
         <v>0</v>
       </c>
-      <c r="J57" s="14" t="s">
+      <c r="J57" s="9" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2252,7 +2249,7 @@
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="16">
+      <c r="I65" s="14">
         <v>1</v>
       </c>
       <c r="J65" s="9"/>
@@ -2744,7 +2741,7 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
-      <c r="E97" s="11" t="s">
+      <c r="E97" s="15" t="s">
         <v>123</v>
       </c>
       <c r="F97" s="4"/>
@@ -2765,9 +2762,9 @@
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="6">
-        <v>0</v>
-      </c>
-      <c r="J98" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="J98" s="16"/>
     </row>
     <row r="99" ht="14.25">
       <c r="A99" s="4"/>
@@ -2812,47 +2809,51 @@
       <c r="J101" s="9"/>
     </row>
     <row r="102" ht="14.25">
-      <c r="A102" s="11"/>
-      <c r="B102" s="11"/>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11" t="s">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
+      <c r="H102" s="4"/>
+      <c r="I102" s="6">
+        <v>1</v>
+      </c>
+      <c r="J102" s="9"/>
+    </row>
+    <row r="103" ht="14.25">
+      <c r="A103" s="4"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="4"/>
+      <c r="E103" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
-      <c r="I102" s="13"/>
-      <c r="J102" s="10"/>
-    </row>
-    <row r="103" ht="14.25">
-      <c r="A103" s="11"/>
-      <c r="B103" s="11"/>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
-      <c r="I103" s="13">
-        <v>0</v>
-      </c>
-      <c r="J103" s="10"/>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
+      <c r="I103" s="6">
+        <v>1</v>
+      </c>
+      <c r="J103" s="9"/>
     </row>
     <row r="104" ht="14.25">
       <c r="A104" s="4"/>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
-      <c r="E104" s="4"/>
-      <c r="F104" s="4" t="s">
-        <v>125</v>
-      </c>
+      <c r="E104" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
-      <c r="I104" s="6"/>
+      <c r="I104" s="6">
+        <v>1</v>
+      </c>
       <c r="J104" s="9"/>
     </row>
     <row r="105" ht="14.25">
@@ -2862,11 +2863,13 @@
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
-      <c r="I105" s="6"/>
+      <c r="I105" s="6">
+        <v>1</v>
+      </c>
       <c r="J105" s="9"/>
     </row>
     <row r="106" ht="14.25">
@@ -2876,22 +2879,23 @@
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
       <c r="F106" s="4" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
-      <c r="I106" s="6"/>
+      <c r="I106" s="6">
+        <v>1</v>
+      </c>
       <c r="J106" s="9"/>
     </row>
     <row r="107" ht="14.25">
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
-      <c r="D107" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="F107" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="6">
@@ -2903,10 +2907,10 @@
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
-      <c r="E108" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="D108" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E108" s="4"/>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
@@ -2921,7 +2925,7 @@
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
@@ -2936,10 +2940,10 @@
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
-      <c r="F110" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="E110" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
       <c r="I110" s="6">
@@ -2950,32 +2954,29 @@
     <row r="111" ht="14.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="4"/>
+      <c r="C111" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
-      <c r="F111" s="4" t="s">
-        <v>130</v>
-      </c>
+      <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
-      <c r="I111" s="6">
-        <v>1</v>
-      </c>
+      <c r="I111" s="6"/>
       <c r="J111" s="9"/>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
-      <c r="D112" s="4"/>
-      <c r="F112" s="4" t="s">
-        <v>131</v>
-      </c>
+      <c r="D112" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
-      <c r="I112" s="6">
-        <v>1</v>
-      </c>
+      <c r="I112" s="6"/>
       <c r="J112" s="9"/>
     </row>
     <row r="113" ht="14.25">
@@ -2983,55 +2984,49 @@
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
-      <c r="I113" s="6">
-        <v>1</v>
-      </c>
+      <c r="I113" s="6"/>
       <c r="J113" s="9"/>
     </row>
     <row r="114" ht="14.25">
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
-      <c r="D114" s="4"/>
-      <c r="E114" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D114" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E114" s="4"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
-      <c r="I114" s="6">
-        <v>1</v>
-      </c>
+      <c r="I114" s="6"/>
       <c r="J114" s="9"/>
     </row>
     <row r="115" ht="14.25">
       <c r="A115" s="4"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
-      <c r="D115" s="4"/>
-      <c r="E115" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="D115" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E115" s="4"/>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
-      <c r="I115" s="6">
-        <v>1</v>
-      </c>
+      <c r="I115" s="6"/>
       <c r="J115" s="9"/>
     </row>
     <row r="116" ht="14.25">
       <c r="A116" s="4"/>
-      <c r="B116" s="4"/>
-      <c r="C116" s="4" t="s">
-        <v>134</v>
-      </c>
+      <c r="B116" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
@@ -3043,154 +3038,89 @@
     <row r="117" ht="14.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4" t="s">
-        <v>135</v>
-      </c>
+      <c r="C117" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D117" s="4"/>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="6"/>
-      <c r="J117" s="9"/>
+      <c r="J117" s="9" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="118" ht="14.25">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
-      <c r="C118" s="4"/>
-      <c r="D118" s="4" t="s">
-        <v>136</v>
-      </c>
+      <c r="C118" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D118" s="4"/>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
       <c r="I118" s="6"/>
-      <c r="J118" s="9"/>
+      <c r="J118" s="9" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="119" ht="14.25">
       <c r="A119" s="4"/>
-      <c r="B119" s="4"/>
+      <c r="B119" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="C119" s="4"/>
-      <c r="D119" s="4" t="s">
-        <v>137</v>
-      </c>
+      <c r="D119" s="4"/>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
-      <c r="H119" s="4"/>
+      <c r="H119" s="17"/>
       <c r="I119" s="6"/>
-      <c r="J119" s="9"/>
-    </row>
-    <row r="120" ht="14.25">
-      <c r="A120" s="4"/>
-      <c r="B120" s="4"/>
-      <c r="C120" s="4"/>
-      <c r="D120" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
-      <c r="G120" s="4"/>
-      <c r="H120" s="4"/>
+      <c r="J119" s="18"/>
+    </row>
+    <row r="120" ht="28.5">
+      <c r="C120" t="s">
+        <v>142</v>
+      </c>
       <c r="I120" s="6"/>
-      <c r="J120" s="9"/>
+      <c r="J120" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="121" ht="14.25">
-      <c r="A121" s="4"/>
-      <c r="B121" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C121" s="4"/>
-      <c r="D121" s="4"/>
-      <c r="E121" s="4"/>
-      <c r="F121" s="4"/>
-      <c r="G121" s="4"/>
-      <c r="H121" s="4"/>
+      <c r="B121" t="s">
+        <v>144</v>
+      </c>
+      <c r="C121" s="19"/>
       <c r="I121" s="6"/>
-      <c r="J121" s="9"/>
+      <c r="J121" s="19"/>
     </row>
     <row r="122" ht="14.25">
-      <c r="A122" s="4"/>
-      <c r="B122" s="4"/>
-      <c r="C122" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D122" s="4"/>
-      <c r="E122" s="4"/>
-      <c r="F122" s="4"/>
-      <c r="G122" s="4"/>
-      <c r="H122" s="4"/>
+      <c r="C122" t="s">
+        <v>145</v>
+      </c>
       <c r="I122" s="6"/>
-      <c r="J122" s="9" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="123" ht="14.25">
-      <c r="A123" s="4"/>
-      <c r="B123" s="4"/>
-      <c r="C123" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D123" s="4"/>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
-      <c r="G123" s="4"/>
-      <c r="H123" s="4"/>
+      <c r="C123" t="s">
+        <v>146</v>
+      </c>
       <c r="I123" s="6"/>
-      <c r="J123" s="9" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="124" ht="14.25">
-      <c r="A124" s="4"/>
-      <c r="B124" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C124" s="4"/>
-      <c r="D124" s="4"/>
-      <c r="E124" s="4"/>
-      <c r="F124" s="4"/>
-      <c r="G124" s="4"/>
-      <c r="H124" s="17"/>
+      <c r="C124" t="s">
+        <v>94</v>
+      </c>
       <c r="I124" s="6"/>
-      <c r="J124" s="18"/>
-    </row>
-    <row r="125" ht="28.5">
-      <c r="C125" t="s">
-        <v>143</v>
-      </c>
-      <c r="I125" s="6"/>
-      <c r="J125" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="126" ht="14.25">
-      <c r="B126" t="s">
-        <v>145</v>
-      </c>
-      <c r="C126" s="19"/>
-      <c r="I126" s="6"/>
-      <c r="J126" s="19"/>
-    </row>
-    <row r="127" ht="14.25">
-      <c r="C127" t="s">
-        <v>146</v>
-      </c>
-      <c r="I127" s="6"/>
-    </row>
-    <row r="128" ht="14.25">
-      <c r="C128" t="s">
-        <v>147</v>
-      </c>
-      <c r="I128" s="6"/>
-    </row>
-    <row r="129" ht="14.25">
-      <c r="C129" t="s">
-        <v>94</v>
-      </c>
-      <c r="I129" s="6"/>
-    </row>
+    </row>
+    <row r="125" ht="28.5"/>
+    <row r="126" ht="14.25"/>
+    <row r="127" ht="14.25"/>
+    <row r="128" ht="14.25"/>
+    <row r="129" ht="14.25"/>
     <row r="130" ht="14.25"/>
     <row r="131" ht="14.25"/>
     <row r="132" ht="14.25"/>
@@ -3214,7 +3144,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008D00AC-00F0-4533-A424-001A00C800AC}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0027006C-005D-47B0-ACD1-00650064004F}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3228,10 +3158,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I107 I109:I120 I46:I49</xm:sqref>
+          <xm:sqref>I3:I102 I104:I115 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00B00071-0006-4F72-AD5B-0052008E00DB}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{001E0008-0076-4063-899E-002C009E00AF}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3245,10 +3175,197 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I122</xm:sqref>
+          <xm:sqref>I117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D700E0-00A9-4879-B4E1-0006003200A1}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00B60056-00EA-4F54-8B38-0081002A00E5}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I116</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007A00FB-0058-4478-8A78-00EF0004001C}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00370034-0081-46BB-B339-0059000C0036}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I27</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00810050-00CA-4079-8ADC-007300850046}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{002D0031-00BD-4C05-86C8-004600960015}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D800CF-0088-4025-B2E3-00B100CD009E}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005F00B5-007C-4C93-A81B-00E300970091}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00650081-008F-467E-92DF-00E200C900D4}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I66</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D10068-00DB-4507-89A6-0007001A00FD}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I119</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004D00B0-001E-4DC4-B367-007F00A600D9}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I120</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00C80034-0038-4141-BE21-00CC006D00E9}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I103</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00F400E4-00AF-477A-A550-004200D100E0}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3265,194 +3382,7 @@
           <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00BA0092-00D2-47CA-B9B6-000D0041004F}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E80081-00AD-4C2B-B86B-005F003D003A}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0041008E-001B-4A28-9BA8-009A001D003B}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007B00FD-002E-4A8F-BCA7-008000CB002D}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I44</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{009E00F4-00B0-48F2-B3BA-007600A40073}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I68</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008800FF-009D-4228-B8C3-000700FC006F}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I67</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{006A008F-00A4-42CD-93B9-005F0097000C}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I66</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00480076-00AA-45BD-9D25-00D100310035}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I124</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007D006D-0047-429D-8EA9-005200F7005C}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I125</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0035008F-0046-4C52-A378-00FB000C00F4}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I108</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00F100DB-0029-4F88-88D8-008B000500F7}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I126</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000600B5-00A4-412C-9EA3-00E3006D0061}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C90043-002E-4C62-887C-008A001C0026}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3469,7 +3399,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{001E0066-001D-4CF2-87CA-0088004200B2}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000100E7-0001-4C5F-91AE-002200F80057}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3483,10 +3413,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I122</xm:sqref>
+          <xm:sqref>I117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B60097-0032-43D0-8AD0-002400750070}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{009900FC-009B-40CC-ABF1-00DB00F600C5}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3500,10 +3430,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I107 I109:I120 I46:I49</xm:sqref>
+          <xm:sqref>I3:I102 I104:I115 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{009E00DA-0033-4A81-824C-0005006E00A3}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{005600C1-0011-4C75-89D7-005A000700F2}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3520,7 +3450,160 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{007D0021-00A4-4803-9D69-009C00860058}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003E0009-009D-481E-BBF3-009800060017}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I116</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001B00BC-001B-4EFD-975E-0063002C00A0}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00FB0054-008F-4B3C-AC37-00DA009900AD}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I44</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B30060-009D-4278-8C1A-00F400D20092}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I68</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00570004-000F-4244-A0B0-00F9003E0058}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I67</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C30076-0053-4CA7-9220-000800A8003A}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I66</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00160083-00FB-4499-BD96-008F00C10029}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I119</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00320008-003B-4A8A-BBC4-00D6009A0049}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I120</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003D007A-006E-48DC-B75D-0075002E0072}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I103</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0023005F-0091-4064-939C-00D900D600AF}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3537,160 +3620,7 @@
           <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{004A0045-00BC-441A-B065-0000008B001F}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00D40081-00E9-45CB-9516-00690040008C}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I44</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003B00F4-0049-41E1-9B60-00B500DA00BA}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I68</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00740022-0032-496B-89BE-00E6008400C3}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I67</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C90073-00AC-483C-ADC2-00A200DC0049}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I66</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{005700B3-00F1-436A-BC8E-00B1007400F0}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I124</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{008E0091-00F4-47D0-8359-0083005200E1}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I125</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B50020-00D7-488C-A7ED-00A800700049}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I108</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00630059-0073-4D81-B929-0056003C00D8}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I126</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00070097-00D4-41D6-8F82-00E600190043}">
+          <x14:cfRule type="dataBar" priority="2" id="{001100D2-00C6-44EC-A2BA-00C400D300C2}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3706,7 +3636,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00610019-00BB-4275-BD7E-005700DC00C2}">
+          <x14:cfRule type="dataBar" priority="1" id="{00FB0003-00D3-49B4-AC7A-00C900C8009E}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
grapple targets fixed: de-parented from Earth
</commit_message>
<xml_diff>
--- a/SatManager Work Breakdown Structure.xlsx
+++ b/SatManager Work Breakdown Structure.xlsx
@@ -597,7 +597,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -638,12 +638,6 @@
     </xf>
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1242,7 +1236,7 @@
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f>COUNTIF(I2:I115,"0")/ROWS(Table5[])</f>
-        <v>2.4390243902439025e-002</v>
+        <v>3.2520325203252036e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -2741,7 +2735,7 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
-      <c r="E97" s="15" t="s">
+      <c r="E97" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F97" s="4"/>
@@ -2764,7 +2758,7 @@
       <c r="I98" s="6">
         <v>1</v>
       </c>
-      <c r="J98" s="16"/>
+      <c r="J98" s="9"/>
     </row>
     <row r="99" ht="14.25">
       <c r="A99" s="4"/>
@@ -2777,7 +2771,9 @@
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
-      <c r="I99" s="6"/>
+      <c r="I99" s="6">
+        <v>0</v>
+      </c>
       <c r="J99" s="9"/>
     </row>
     <row r="100" ht="14.25">
@@ -3077,9 +3073,9 @@
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
-      <c r="H119" s="17"/>
+      <c r="H119" s="15"/>
       <c r="I119" s="6"/>
-      <c r="J119" s="18"/>
+      <c r="J119" s="16"/>
     </row>
     <row r="120" ht="28.5">
       <c r="C120" t="s">
@@ -3094,9 +3090,9 @@
       <c r="B121" t="s">
         <v>144</v>
       </c>
-      <c r="C121" s="19"/>
+      <c r="C121" s="17"/>
       <c r="I121" s="6"/>
-      <c r="J121" s="19"/>
+      <c r="J121" s="17"/>
     </row>
     <row r="122" ht="14.25">
       <c r="C122" t="s">
@@ -3144,7 +3140,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0027006C-005D-47B0-ACD1-00650064004F}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{004900C6-004F-4CFD-AC7C-001D005E008D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3161,7 +3157,7 @@
           <xm:sqref>I3:I102 I104:I115 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{001E0008-0076-4063-899E-002C009E00AF}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005800F5-0059-4CFF-85C1-00E100700079}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3178,7 +3174,7 @@
           <xm:sqref>I117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00B60056-00EA-4F54-8B38-0081002A00E5}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{006F009C-0012-4C0E-A8CD-0073005400FC}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3195,7 +3191,7 @@
           <xm:sqref>I116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007A00FB-0058-4478-8A78-00EF0004001C}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003C0003-008B-454E-A2BF-00A0009C000E}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3212,7 +3208,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00370034-0081-46BB-B339-0059000C0036}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007600C2-00BF-4597-957C-0045007C001F}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3229,7 +3225,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00810050-00CA-4079-8ADC-007300850046}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00540046-0007-4FF4-9627-00D7004F0091}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3246,7 +3242,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{002D0031-00BD-4C05-86C8-004600960015}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00130051-00A4-4227-9BAC-00DC00120039}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3263,7 +3259,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D800CF-0088-4025-B2E3-00B100CD009E}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00730076-0039-4923-BD3B-006F00E700E1}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3280,7 +3276,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{005F00B5-007C-4C93-A81B-00E300970091}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003A00A1-004D-4591-80C4-00C0009400C9}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3297,7 +3293,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00650081-008F-467E-92DF-00E200C900D4}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00B0008D-00CE-404C-B980-009100020021}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3314,7 +3310,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D10068-00DB-4507-89A6-0007001A00FD}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0022004C-0089-4EE4-B669-00BA00BE0091}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3331,7 +3327,7 @@
           <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{004D00B0-001E-4DC4-B367-007F00A600D9}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{006000C2-00B3-481F-80BE-00A6007B00B2}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3348,7 +3344,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C80034-0038-4141-BE21-00CC006D00E9}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003F002A-0063-4873-AA80-00D4008E0092}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3365,7 +3361,7 @@
           <xm:sqref>I103</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00F400E4-00AF-477A-A550-004200D100E0}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00170090-0015-468D-ACF8-005700710033}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3382,7 +3378,7 @@
           <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C90043-002E-4C62-887C-008A001C0026}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00450056-0029-47CE-972F-00560041000C}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3399,7 +3395,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000100E7-0001-4C5F-91AE-002200F80057}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00AA00AF-0062-44C8-8C72-008D003F0087}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3416,7 +3412,7 @@
           <xm:sqref>I117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{009900FC-009B-40CC-ABF1-00DB00F600C5}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{002A0026-0068-4DC6-92D7-00CA00520082}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3433,7 +3429,7 @@
           <xm:sqref>I3:I102 I104:I115 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{005600C1-0011-4C75-89D7-005A000700F2}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{002F0018-0046-4F41-B1B3-0071008400CE}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3450,7 +3446,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003E0009-009D-481E-BBF3-009800060017}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00240036-00EC-466B-A022-00F8008100B3}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3467,7 +3463,7 @@
           <xm:sqref>I116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{001B00BC-001B-4EFD-975E-0063002C00A0}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00FA0005-00AE-45A9-8380-006B001B006A}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3484,7 +3480,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00FB0054-008F-4B3C-AC37-00DA009900AD}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00A6005E-00C4-4910-BDF0-00EA00C900A1}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3501,7 +3497,7 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B30060-009D-4278-8C1A-00F400D20092}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00A000ED-00C8-4AEF-8CDB-0026002300FB}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3518,7 +3514,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00570004-000F-4244-A0B0-00F9003E0058}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{006600B6-003B-4846-B76B-00E80067008D}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3535,7 +3531,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C30076-0053-4CA7-9220-000800A8003A}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00F7008B-0000-4547-8D0C-008A00F70062}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3552,7 +3548,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00160083-00FB-4499-BD96-008F00C10029}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00590097-00DE-41DC-B3F5-007B00D900F8}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3569,7 +3565,7 @@
           <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00320008-003B-4A8A-BBC4-00D6009A0049}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001300D7-0003-4E20-8799-00BF003600C1}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3586,7 +3582,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003D007A-006E-48DC-B75D-0075002E0072}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B3009C-007C-4EE4-8732-006D00DB00A2}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3603,7 +3599,7 @@
           <xm:sqref>I103</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0023005F-0091-4064-939C-00D900D600AF}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{004A000A-00BE-422C-9442-003000BB0077}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3620,7 +3616,7 @@
           <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{001100D2-00C6-44EC-A2BA-00C400D300C2}">
+          <x14:cfRule type="dataBar" priority="2" id="{00EB009C-0020-43AF-810B-00C7006B008E}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3636,7 +3632,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00FB0003-00D3-49B4-AC7A-00C900C8009E}">
+          <x14:cfRule type="dataBar" priority="1" id="{0030009E-005F-415B-AF12-008400A50028}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
updated colors, added money & launch cost
</commit_message>
<xml_diff>
--- a/SatManager Work Breakdown Structure.xlsx
+++ b/SatManager Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>Status</t>
   </si>
@@ -252,6 +252,9 @@
     <t xml:space="preserve">set all parameters to match grabbler</t>
   </si>
   <si>
+    <t>test</t>
+  </si>
+  <si>
     <t>maneuver</t>
   </si>
   <si>
@@ -324,12 +327,6 @@
     <t xml:space="preserve">probability to destroy satellite</t>
   </si>
   <si>
-    <t xml:space="preserve">other satellites</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chance to put a satellite in a random orbit. can view tlm but no control</t>
-  </si>
-  <si>
     <t xml:space="preserve">space wx</t>
   </si>
   <si>
@@ -435,10 +432,10 @@
     <t xml:space="preserve">80/90s asthetic - win95 style</t>
   </si>
   <si>
-    <t>lighting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dark side of earth needs to be visible</t>
+    <t xml:space="preserve">earth texture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low-poly, low-res map</t>
   </si>
   <si>
     <t xml:space="preserve">Refactor/Performance Pass</t>
@@ -639,11 +636,11 @@
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1182,7 +1179,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1236,13 +1233,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.48780487804878048</v>
+        <v>0.51219512195121952</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f>COUNTIF(I2:I115,"0")/ROWS(Table5[])</f>
-        <v>4.878048780487805e-002</v>
+        <v>0</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1314,7 +1311,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1664,7 +1661,9 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="6"/>
+      <c r="I30" s="6">
+        <v>1</v>
+      </c>
       <c r="J30" s="9" t="s">
         <v>35</v>
       </c>
@@ -1746,7 +1745,9 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-      <c r="I35" s="6"/>
+      <c r="I35" s="6">
+        <v>1</v>
+      </c>
       <c r="J35" s="9" t="s">
         <v>43</v>
       </c>
@@ -1826,9 +1827,7 @@
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
-      <c r="I40" s="6">
-        <v>0</v>
-      </c>
+      <c r="I40" s="6"/>
       <c r="J40" s="9"/>
     </row>
     <row r="41" ht="14.25">
@@ -1907,9 +1906,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="6">
-        <v>0</v>
-      </c>
+      <c r="I45" s="6"/>
       <c r="J45" s="9"/>
     </row>
     <row r="46" ht="14.25">
@@ -2011,9 +2008,7 @@
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
-      <c r="I51" s="6">
-        <v>0</v>
-      </c>
+      <c r="I51" s="6"/>
       <c r="J51" s="9" t="s">
         <v>67</v>
       </c>
@@ -2083,9 +2078,7 @@
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
-      <c r="I55" s="6">
-        <v>0</v>
-      </c>
+      <c r="I55" s="6"/>
       <c r="J55" s="9"/>
     </row>
     <row r="56" ht="14.25">
@@ -2099,9 +2092,7 @@
         <v>75</v>
       </c>
       <c r="H56" s="4"/>
-      <c r="I56" s="6">
-        <v>0</v>
-      </c>
+      <c r="I56" s="6"/>
       <c r="J56" s="9" t="s">
         <v>76</v>
       </c>
@@ -2118,7 +2109,7 @@
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J57" s="9" t="s">
         <v>78</v>
@@ -2129,15 +2120,13 @@
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
       <c r="H58" s="4"/>
-      <c r="I58" s="6">
-        <v>1</v>
-      </c>
+      <c r="I58" s="6"/>
       <c r="J58" s="9"/>
     </row>
     <row r="59" ht="28.5">
@@ -2145,18 +2134,16 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E59" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F59" s="4"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="6">
         <v>1</v>
       </c>
-      <c r="J59" s="9" t="s">
-        <v>80</v>
-      </c>
+      <c r="J59" s="9"/>
     </row>
     <row r="60" ht="28.5">
       <c r="A60" s="4"/>
@@ -2165,7 +2152,7 @@
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
@@ -2173,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" ht="28.5">
@@ -2183,7 +2170,7 @@
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
@@ -2191,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" ht="14.25">
@@ -2199,17 +2186,17 @@
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
-      <c r="E62" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="6">
         <v>1</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" ht="14.25">
@@ -2218,7 +2205,7 @@
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -2227,7 +2214,7 @@
         <v>1</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" ht="28.5">
@@ -2236,7 +2223,7 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2245,24 +2232,26 @@
         <v>1</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" ht="14.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
-      <c r="D65" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="14">
-        <v>1</v>
-      </c>
-      <c r="J65" s="9"/>
+      <c r="I65" s="6">
+        <v>1</v>
+      </c>
+      <c r="J65" s="9" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="66" ht="14.25">
       <c r="A66" s="4"/>
@@ -2275,7 +2264,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
-      <c r="I66" s="6">
+      <c r="I66" s="15">
         <v>1</v>
       </c>
       <c r="J66" s="9"/>
@@ -2284,10 +2273,10 @@
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4" t="s">
+      <c r="D67" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
@@ -2315,11 +2304,11 @@
     <row r="69" ht="14.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
@@ -2331,10 +2320,10 @@
     <row r="70" ht="14.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -2342,47 +2331,49 @@
       <c r="I70" s="6">
         <v>1</v>
       </c>
-      <c r="J70" s="9" t="s">
-        <v>97</v>
-      </c>
+      <c r="J70" s="9"/>
     </row>
     <row r="71" ht="14.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
-      <c r="I71" s="6"/>
+      <c r="I71" s="6">
+        <v>1</v>
+      </c>
       <c r="J71" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="6"/>
-      <c r="J72" s="9"/>
+      <c r="J72" s="9" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="73" ht="14.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4" t="s">
+      <c r="C73" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="D73" s="4"/>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
@@ -2394,10 +2385,10 @@
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="D74" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
@@ -2410,7 +2401,7 @@
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -2419,27 +2410,25 @@
       <c r="J75" s="9"/>
     </row>
     <row r="76" ht="28.5">
-      <c r="A76" s="11"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11" t="s">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="10" t="s">
-        <v>104</v>
-      </c>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="9"/>
     </row>
     <row r="77" ht="28.5">
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
@@ -2454,7 +2443,7 @@
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
@@ -2468,7 +2457,7 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -2510,7 +2499,7 @@
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -2524,7 +2513,7 @@
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
@@ -2536,7 +2525,7 @@
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -2553,7 +2542,7 @@
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
@@ -2563,7 +2552,7 @@
         <v>1</v>
       </c>
       <c r="J85" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="86" ht="14.25">
@@ -2571,7 +2560,7 @@
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
@@ -2581,7 +2570,7 @@
         <v>1</v>
       </c>
       <c r="J86" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="87" ht="14.25">
@@ -2607,7 +2596,7 @@
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
       <c r="F88" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
@@ -2623,7 +2612,7 @@
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
@@ -2639,7 +2628,7 @@
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
@@ -2655,7 +2644,7 @@
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
       <c r="F91" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
@@ -2670,7 +2659,7 @@
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
@@ -2679,7 +2668,7 @@
         <v>1</v>
       </c>
       <c r="J92" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="93" ht="14.25">
@@ -2689,7 +2678,7 @@
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -2705,7 +2694,7 @@
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
@@ -2721,7 +2710,7 @@
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
       <c r="F95" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
@@ -2737,7 +2726,7 @@
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
@@ -2752,7 +2741,7 @@
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
@@ -2769,7 +2758,7 @@
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
       <c r="F98" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
@@ -2785,15 +2774,15 @@
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="6">
         <v>1</v>
       </c>
-      <c r="J99" s="15" t="s">
-        <v>126</v>
+      <c r="J99" s="9" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="100" ht="14.25">
@@ -2803,7 +2792,7 @@
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
       <c r="F100" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
@@ -2819,7 +2808,7 @@
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
       <c r="F101" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
@@ -2850,7 +2839,7 @@
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
@@ -2866,7 +2855,7 @@
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
@@ -2883,7 +2872,7 @@
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
@@ -2899,7 +2888,7 @@
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
       <c r="F106" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
@@ -2914,7 +2903,7 @@
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
       <c r="F107" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
@@ -2928,7 +2917,7 @@
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E108" s="4"/>
       <c r="F108" s="4"/>
@@ -2961,7 +2950,7 @@
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
@@ -2975,7 +2964,7 @@
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
       <c r="C111" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -2990,7 +2979,7 @@
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
@@ -3004,7 +2993,7 @@
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
@@ -3018,7 +3007,7 @@
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
@@ -3044,7 +3033,7 @@
     <row r="116" ht="14.25">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
@@ -3068,14 +3057,14 @@
       <c r="H117" s="4"/>
       <c r="I117" s="6"/>
       <c r="J117" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="118" ht="14.25">
       <c r="A118" s="4"/>
       <c r="B118" s="4"/>
       <c r="C118" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -3084,13 +3073,13 @@
       <c r="H118" s="4"/>
       <c r="I118" s="6"/>
       <c r="J118" s="9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="119" ht="14.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="119" ht="28.5">
       <c r="A119" s="4"/>
       <c r="B119" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
@@ -3103,16 +3092,16 @@
     </row>
     <row r="120" ht="28.5">
       <c r="C120" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I120" s="6"/>
       <c r="J120" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="121" ht="28.5">
       <c r="B121" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C121" s="18"/>
       <c r="I121" s="6"/>
@@ -3120,19 +3109,19 @@
     </row>
     <row r="122" ht="14.25">
       <c r="C122" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I122" s="6"/>
     </row>
     <row r="123" ht="14.25">
       <c r="C123" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I123" s="6"/>
     </row>
     <row r="124" ht="14.25">
       <c r="C124" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I124" s="6"/>
     </row>
@@ -3164,7 +3153,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{000C003F-0049-4F46-A702-00B8002B000C}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00140028-0061-4081-939A-003200B60096}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3181,7 +3170,7 @@
           <xm:sqref>I3:I102 I104:I115 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{003D007E-007D-480D-8A4D-0046009A0088}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00F600E3-0084-452B-8C50-007B00F1003C}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3198,7 +3187,7 @@
           <xm:sqref>I117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0071002D-00D8-4A05-A5C8-001F007B00AF}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00500018-000F-42F2-BFAD-006E00C400DB}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3215,7 +3204,7 @@
           <xm:sqref>I116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{004900EC-00A4-4E92-85D3-00FA006800CE}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00590088-0043-40EE-BB7E-009B00D60066}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3232,7 +3221,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C9008F-0071-45B1-99F0-008000FD0086}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007F003B-00F2-4457-A389-0097001F00B6}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3249,7 +3238,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D7009F-008F-4670-AF42-00D0005B004D}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E100FC-0003-4B0B-BE01-007A006C0006}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3266,7 +3255,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00BF00D7-0097-4F72-BB15-00FC00A600EB}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00D300D9-00F2-460D-900F-006200DE0076}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3283,7 +3272,24 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00B200A8-00E3-4770-B554-008B008800FE}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005E00A4-004D-4401-8A55-00EE006B0088}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I69</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00BD0074-0038-4BB1-8561-00C3005B00A6}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3300,7 +3306,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{004200B5-0011-4DB3-8314-00F500AB0077}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E00024-00E9-468A-8E3C-000B00CC009A}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3317,24 +3323,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E80058-0084-4A9C-B109-002A0042001B}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I66</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007F001B-00E2-401C-BE0C-000B00810002}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00ED00D2-002C-4B20-82E1-00F1002E0014}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3351,7 +3340,7 @@
           <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00C60040-0097-4A3C-B59C-00EF0020001B}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00BA0062-00E0-47A6-BEBA-002600C80027}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3368,7 +3357,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E1003A-0051-4F96-9A59-001F00DD00A7}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005500F9-0079-4C76-972D-0060003200CC}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3385,7 +3374,7 @@
           <xm:sqref>I103</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D80031-0083-41DA-A08B-005B00F700B9}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007C0082-007C-468F-A80C-00D500D8005E}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3402,7 +3391,7 @@
           <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00170082-00E2-4E4A-B899-005300B300BD}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0025002C-0006-4A12-B027-00C4007E001D}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3419,7 +3408,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00EC003C-00EB-4E3E-A992-002E00DB00ED}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00F700EA-0046-4CC5-BDB7-00EC00B600AB}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3436,7 +3425,7 @@
           <xm:sqref>I117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000D00A5-005A-47A0-BBA7-0007003A00DD}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00CF00F2-00FE-4090-AAF0-0013006B0092}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3453,7 +3442,7 @@
           <xm:sqref>I3:I102 I104:I115 I46:I49</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000F00B3-00B4-4D71-B2AF-006B002100F1}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003C003F-0006-4E03-AA78-0081005A00BC}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3470,7 +3459,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F00093-00BF-4043-98A2-00DC00E500E2}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0003000F-00C8-4ECD-A3EA-0082009400F9}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3487,7 +3476,7 @@
           <xm:sqref>I116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{008E0025-0005-4EBD-981E-0051005E003C}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{009C0065-00C5-4846-A053-00E800FD007D}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3504,7 +3493,7 @@
           <xm:sqref>I28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{002D007E-0054-461B-A6E4-00B4006A00E3}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B40088-000F-45E6-86B5-008600D0005F}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3521,7 +3510,24 @@
           <xm:sqref>I44</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F60065-0040-42AB-805B-006300680089}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00A90082-00CD-43CC-A887-00B60018001B}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I69</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001000A2-00BA-4938-9E32-00D400380010}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3538,7 +3544,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{007200D7-00A0-4050-B00D-00AF00BE0039}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003200FB-00A6-4311-B395-00C100650003}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3555,24 +3561,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00130083-000D-4B03-AC27-0060005400D0}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I66</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00AB004E-0067-4F4D-BFF9-002E0016007F}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{008A00E2-00F3-4E60-A483-00610027009A}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3589,7 +3578,7 @@
           <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F300CF-004F-4ACE-867C-004A0076004A}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00490074-001A-42D3-A940-001D00DC00E2}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3606,7 +3595,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000500D4-00AD-4CB9-B4C7-00D300E7008C}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D3000E-0024-4D3B-9307-0062003400CA}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3623,7 +3612,7 @@
           <xm:sqref>I103</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00E300DC-002C-4656-B496-006100630071}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{004000D3-0031-4A0E-B888-002000B600A6}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3640,7 +3629,7 @@
           <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00EE009B-00B9-4B7F-8ECF-007E00E6007A}">
+          <x14:cfRule type="dataBar" priority="2" id="{00DC002A-00F4-4FE6-B262-004B003900AD}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3656,7 +3645,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{006F007A-0008-4323-A5F5-002800F000FC}">
+          <x14:cfRule type="dataBar" priority="1" id="{00A7003C-0034-4A00-A7AD-005E006C007B}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
started save & pause menu, cleaned old files
</commit_message>
<xml_diff>
--- a/SatManager Work Breakdown Structure.xlsx
+++ b/SatManager Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>Status</t>
   </si>
@@ -72,9 +72,6 @@
     <t>resolution</t>
   </si>
   <si>
-    <t>units</t>
-  </si>
-  <si>
     <t>quit</t>
   </si>
   <si>
@@ -310,12 +307,6 @@
   </si>
   <si>
     <t xml:space="preserve">right-mouse &amp; drag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">switch focus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">satellites or earth</t>
   </si>
   <si>
     <t xml:space="preserve">event system</t>
@@ -597,7 +588,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -636,11 +627,14 @@
     <xf fontId="0" fillId="5" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -669,7 +663,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J124" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J123" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1179,7 +1173,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A62" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1233,13 +1227,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.51219512195121952</v>
+        <v>0.52459016393442626</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I115,"0")/ROWS(Table5[])</f>
-        <v>0</v>
+        <f>COUNTIF(I2:I114,"0")/ROWS(Table5[])</f>
+        <v>1.6393442622950821e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1255,7 +1249,9 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="6"/>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
       <c r="J3" s="9"/>
       <c r="L3" t="s">
         <v>6</v>
@@ -1272,11 +1268,13 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="6"/>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1311,7 +1309,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -1458,10 +1456,10 @@
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -1472,10 +1470,10 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -1488,7 +1486,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1499,11 +1497,11 @@
     <row r="20" ht="14.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -1526,10 +1524,10 @@
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -1538,68 +1536,72 @@
       <c r="I22" s="6"/>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" ht="14.25">
+    <row r="23" ht="28.5">
       <c r="A23" s="4"/>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="9"/>
+      <c r="I23" s="6">
+        <v>1</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" ht="28.5">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="6">
-        <v>1</v>
-      </c>
+      <c r="I24" s="6"/>
       <c r="J24" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" ht="28.5">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="6"/>
       <c r="J25" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" ht="28.5">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="C26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="6"/>
+      <c r="I26" s="6">
+        <v>1</v>
+      </c>
       <c r="J26" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" ht="14.25">
@@ -1616,9 +1618,7 @@
       <c r="I27" s="6">
         <v>1</v>
       </c>
-      <c r="J27" s="9" t="s">
-        <v>28</v>
-      </c>
+      <c r="J27" s="9"/>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="4"/>
@@ -1631,31 +1631,33 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="6">
-        <v>1</v>
-      </c>
+      <c r="I28" s="6"/>
       <c r="J28" s="9"/>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="9"/>
+      <c r="I29" s="6">
+        <v>1</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -1665,7 +1667,7 @@
         <v>1</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" ht="28.5">
@@ -1673,7 +1675,7 @@
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -1682,9 +1684,7 @@
       <c r="I31" s="6">
         <v>1</v>
       </c>
-      <c r="J31" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="J31" s="9"/>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="4"/>
@@ -1697,12 +1697,10 @@
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="6">
-        <v>1</v>
-      </c>
+      <c r="I32" s="6"/>
       <c r="J32" s="9"/>
     </row>
-    <row r="33" ht="14.25">
+    <row r="33" ht="28.5">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1713,15 +1711,19 @@
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="9"/>
+      <c r="I33" s="6">
+        <v>1</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="34" ht="28.5">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1730,8 +1732,8 @@
       <c r="I34" s="6">
         <v>1</v>
       </c>
-      <c r="J34" s="10" t="s">
-        <v>41</v>
+      <c r="J34" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="35" ht="14.25">
@@ -1739,32 +1741,30 @@
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-      <c r="I35" s="6">
-        <v>1</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="I35" s="6"/>
+      <c r="J35" s="9"/>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="4"/>
+      <c r="E36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="6"/>
-      <c r="J36" s="9"/>
+      <c r="J36" s="9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="4"/>
@@ -1772,14 +1772,16 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
-      <c r="I37" s="6"/>
+      <c r="I37" s="6">
+        <v>1</v>
+      </c>
       <c r="J37" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" ht="14.25">
@@ -1788,7 +1790,7 @@
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -1796,38 +1798,36 @@
       <c r="I38" s="6">
         <v>1</v>
       </c>
-      <c r="J38" s="9" t="s">
-        <v>48</v>
-      </c>
+      <c r="J38" s="9"/>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="D39" s="4"/>
-      <c r="E39" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
-      <c r="I39" s="6">
-        <v>1</v>
-      </c>
+      <c r="I39" s="6"/>
       <c r="J39" s="9"/>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="4"/>
+      <c r="D40" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
-      <c r="I40" s="6"/>
+      <c r="I40" s="6">
+        <v>1</v>
+      </c>
       <c r="J40" s="9"/>
     </row>
     <row r="41" ht="14.25">
@@ -1837,7 +1837,6 @@
       <c r="D41" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -1850,63 +1849,64 @@
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="6">
+      <c r="I42" s="12">
         <v>1</v>
       </c>
       <c r="J42" s="9"/>
     </row>
     <row r="43" ht="28.5">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4" t="s">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="12">
-        <v>1</v>
-      </c>
-      <c r="J43" s="9"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="13">
+        <v>1</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="44" ht="28.5">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="13">
-        <v>1</v>
-      </c>
-      <c r="J44" s="9" t="s">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="9"/>
     </row>
     <row r="45" ht="14.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="4"/>
+      <c r="E45" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="6"/>
+      <c r="I45" s="6">
+        <v>1</v>
+      </c>
       <c r="J45" s="9"/>
     </row>
     <row r="46" ht="14.25">
@@ -1914,16 +1914,18 @@
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="6">
         <v>1</v>
       </c>
-      <c r="J46" s="9"/>
+      <c r="J46" s="9" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="47" ht="28.5">
       <c r="A47" s="4"/>
@@ -1932,7 +1934,7 @@
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
@@ -1940,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" ht="28.5">
@@ -1950,7 +1952,7 @@
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
@@ -1958,43 +1960,41 @@
         <v>1</v>
       </c>
       <c r="J48" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49" ht="14.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="6">
-        <v>1</v>
-      </c>
-      <c r="J49" s="9" t="s">
+    </row>
+    <row r="49" ht="28.5">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="13">
+        <v>1</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="50" ht="28.5">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="13">
-        <v>1</v>
-      </c>
-      <c r="J50" s="10" t="s">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4" t="s">
         <v>65</v>
+      </c>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="51" ht="14.25">
@@ -2002,25 +2002,27 @@
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
-      <c r="E51" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
-      <c r="I51" s="6"/>
+      <c r="I51" s="6">
+        <v>1</v>
+      </c>
       <c r="J51" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" ht="14.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" ht="28.5">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
@@ -2028,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" ht="28.5">
@@ -2038,7 +2040,7 @@
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
@@ -2046,7 +2048,7 @@
         <v>1</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" ht="28.5">
@@ -2056,16 +2058,12 @@
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
-      <c r="I54" s="6">
-        <v>1</v>
-      </c>
-      <c r="J54" s="9" t="s">
-        <v>73</v>
-      </c>
+      <c r="I54" s="6"/>
+      <c r="J54" s="9"/>
     </row>
     <row r="55" ht="14.25">
       <c r="A55" s="4"/>
@@ -2073,13 +2071,17 @@
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="4"/>
+      <c r="G55" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G55" s="4"/>
       <c r="H55" s="4"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="9"/>
+      <c r="I55" s="6">
+        <v>1</v>
+      </c>
+      <c r="J55" s="9" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="56" ht="14.25">
       <c r="A56" s="4"/>
@@ -2089,12 +2091,14 @@
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H56" s="4"/>
-      <c r="I56" s="6"/>
+      <c r="I56" s="6">
+        <v>1</v>
+      </c>
       <c r="J56" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" ht="14.25">
@@ -2105,28 +2109,26 @@
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H57" s="4"/>
-      <c r="I57" s="6">
-        <v>1</v>
-      </c>
-      <c r="J57" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="I57" s="6"/>
+      <c r="J57" s="9"/>
     </row>
     <row r="58" ht="14.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
+      <c r="E58" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="F58" s="4"/>
-      <c r="G58" s="14" t="s">
-        <v>79</v>
-      </c>
+      <c r="G58" s="4"/>
       <c r="H58" s="4"/>
-      <c r="I58" s="6"/>
+      <c r="I58" s="6">
+        <v>1</v>
+      </c>
       <c r="J58" s="9"/>
     </row>
     <row r="59" ht="28.5">
@@ -2134,16 +2136,18 @@
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="6">
         <v>1</v>
       </c>
-      <c r="J59" s="9"/>
+      <c r="J59" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="60" ht="28.5">
       <c r="A60" s="4"/>
@@ -2152,7 +2156,7 @@
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
@@ -2160,7 +2164,7 @@
         <v>1</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" ht="28.5">
@@ -2170,7 +2174,7 @@
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
@@ -2178,25 +2182,25 @@
         <v>1</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="62" ht="14.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" ht="28.5">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4" t="s">
-        <v>84</v>
-      </c>
+      <c r="E62" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F62" s="4"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="6">
         <v>1</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" ht="14.25">
@@ -2205,7 +2209,7 @@
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -2214,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="64" ht="28.5">
@@ -2223,7 +2227,7 @@
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -2232,26 +2236,24 @@
         <v>1</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" ht="14.25">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4" t="s">
-        <v>90</v>
-      </c>
+      <c r="D65" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
-      <c r="I65" s="6">
-        <v>1</v>
-      </c>
-      <c r="J65" s="9" t="s">
-        <v>91</v>
-      </c>
+      <c r="I65" s="14">
+        <v>1</v>
+      </c>
+      <c r="J65" s="9"/>
     </row>
     <row r="66" ht="14.25">
       <c r="A66" s="4"/>
@@ -2264,7 +2266,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
-      <c r="I66" s="15">
+      <c r="I66" s="6">
         <v>1</v>
       </c>
       <c r="J66" s="9"/>
@@ -2273,10 +2275,10 @@
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="4"/>
+      <c r="E67" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
@@ -2304,11 +2306,11 @@
     <row r="69" ht="14.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
+      <c r="C69" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="D69" s="4"/>
-      <c r="E69" s="4" t="s">
-        <v>95</v>
-      </c>
+      <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
@@ -2320,10 +2322,10 @@
     <row r="70" ht="14.25">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="4"/>
+      <c r="D70" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -2331,49 +2333,43 @@
       <c r="I70" s="6">
         <v>1</v>
       </c>
-      <c r="J70" s="9"/>
+      <c r="J70" s="9" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="71" ht="14.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
-      <c r="D71" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="D71" s="15"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
-      <c r="I71" s="6">
-        <v>1</v>
-      </c>
-      <c r="J71" s="9" t="s">
-        <v>98</v>
-      </c>
+      <c r="I71" s="6"/>
+      <c r="J71" s="16"/>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="C72" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D72" s="4"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="6"/>
-      <c r="J72" s="9" t="s">
-        <v>100</v>
-      </c>
+      <c r="J72" s="9"/>
     </row>
     <row r="73" ht="14.25">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
-      <c r="C73" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
@@ -2385,10 +2381,10 @@
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
-      <c r="D74" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
@@ -2401,7 +2397,7 @@
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -2413,10 +2409,10 @@
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4" t="s">
-        <v>103</v>
-      </c>
+      <c r="D76" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E76" s="4"/>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
@@ -2427,10 +2423,10 @@
       <c r="A77" s="4"/>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
-      <c r="D77" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
@@ -2443,7 +2439,7 @@
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
@@ -2457,7 +2453,7 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -2469,10 +2465,10 @@
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="D80" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" s="4"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
@@ -2483,10 +2479,10 @@
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
-      <c r="D81" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
@@ -2499,7 +2495,7 @@
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -2510,24 +2506,26 @@
     <row r="83" ht="14.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
+      <c r="C83" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="D83" s="4"/>
-      <c r="E83" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="E83" s="4"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
-      <c r="I83" s="6"/>
+      <c r="I83" s="6">
+        <v>1</v>
+      </c>
       <c r="J83" s="9"/>
     </row>
     <row r="84" ht="14.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
-      <c r="C84" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D84" s="4"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
@@ -2535,14 +2533,16 @@
       <c r="I84" s="6">
         <v>1</v>
       </c>
-      <c r="J84" s="9"/>
+      <c r="J84" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="85" ht="14.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
@@ -2552,36 +2552,34 @@
         <v>1</v>
       </c>
       <c r="J85" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" ht="14.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
-      <c r="D86" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E86" s="4"/>
+      <c r="D86" s="4"/>
+      <c r="E86" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="6">
         <v>1</v>
       </c>
-      <c r="J86" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="J86" s="9"/>
     </row>
     <row r="87" ht="14.25">
       <c r="A87" s="4"/>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
-      <c r="E87" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F87" s="4"/>
+      <c r="E87" s="4"/>
+      <c r="F87" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="6">
@@ -2596,7 +2594,7 @@
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
       <c r="F88" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
@@ -2612,7 +2610,7 @@
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
@@ -2628,7 +2626,7 @@
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
@@ -2642,34 +2640,34 @@
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="E91" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F91" s="4"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="6">
         <v>1</v>
       </c>
-      <c r="J91" s="9"/>
+      <c r="J91" s="9" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="92" ht="14.25">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
-      <c r="E92" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F92" s="4"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="6">
         <v>1</v>
       </c>
-      <c r="J92" s="9" t="s">
-        <v>119</v>
-      </c>
+      <c r="J92" s="9"/>
     </row>
     <row r="93" ht="14.25">
       <c r="A93" s="4"/>
@@ -2678,7 +2676,7 @@
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -2694,7 +2692,7 @@
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
@@ -2710,7 +2708,7 @@
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
       <c r="F95" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
@@ -2724,10 +2722,10 @@
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
-      <c r="E96" s="4"/>
-      <c r="F96" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="E96" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F96" s="4"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="6">
@@ -2740,10 +2738,10 @@
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
-      <c r="E97" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="6">
@@ -2758,14 +2756,16 @@
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
       <c r="F98" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="6">
         <v>1</v>
       </c>
-      <c r="J98" s="9"/>
+      <c r="J98" s="9" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="99" ht="14.25">
       <c r="A99" s="4"/>
@@ -2774,16 +2774,14 @@
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="6">
         <v>1</v>
       </c>
-      <c r="J99" s="9" t="s">
-        <v>125</v>
-      </c>
+      <c r="J99" s="9"/>
     </row>
     <row r="100" ht="14.25">
       <c r="A100" s="4"/>
@@ -2792,7 +2790,7 @@
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
       <c r="F100" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
@@ -2805,11 +2803,11 @@
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
-      <c r="D101" s="4"/>
+      <c r="D101" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E101" s="4"/>
-      <c r="F101" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="F101" s="4"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="6">
@@ -2821,10 +2819,10 @@
       <c r="A102" s="4"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
-      <c r="D102" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
@@ -2839,7 +2837,7 @@
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
@@ -2854,10 +2852,10 @@
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
-      <c r="E104" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F104" s="4"/>
+      <c r="E104" s="4"/>
+      <c r="F104" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="6">
@@ -2872,7 +2870,7 @@
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
@@ -2886,9 +2884,8 @@
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
-      <c r="E106" s="4"/>
       <c r="F106" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
@@ -2901,10 +2898,11 @@
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="F107" s="4" t="s">
-        <v>130</v>
-      </c>
+      <c r="D107" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="6">
@@ -2916,10 +2914,10 @@
       <c r="A108" s="4"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
-      <c r="D108" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="E108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
@@ -2934,7 +2932,7 @@
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
@@ -2947,26 +2945,24 @@
     <row r="110" ht="14.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
-      <c r="C110" s="4"/>
+      <c r="C110" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="D110" s="4"/>
-      <c r="E110" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="E110" s="4"/>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
-      <c r="I110" s="6">
-        <v>1</v>
-      </c>
+      <c r="I110" s="6"/>
       <c r="J110" s="9"/>
     </row>
     <row r="111" ht="14.25">
       <c r="A111" s="4"/>
       <c r="B111" s="4"/>
-      <c r="C111" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
@@ -2979,7 +2975,7 @@
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E112" s="4"/>
       <c r="F112" s="4"/>
@@ -2993,7 +2989,7 @@
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E113" s="4"/>
       <c r="F113" s="4"/>
@@ -3007,7 +3003,7 @@
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4" t="s">
-        <v>136</v>
+        <v>19</v>
       </c>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
@@ -3018,11 +3014,11 @@
     </row>
     <row r="115" ht="14.25">
       <c r="A115" s="4"/>
-      <c r="B115" s="4"/>
+      <c r="B115" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="C115" s="4"/>
-      <c r="D115" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="D115" s="4"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
@@ -3032,23 +3028,25 @@
     </row>
     <row r="116" ht="14.25">
       <c r="A116" s="4"/>
-      <c r="B116" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C116" s="4"/>
+      <c r="B116" s="4"/>
+      <c r="C116" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
       <c r="I116" s="6"/>
-      <c r="J116" s="9"/>
+      <c r="J116" s="9" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="117" ht="14.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
       <c r="C117" s="4" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -3057,74 +3055,59 @@
       <c r="H117" s="4"/>
       <c r="I117" s="6"/>
       <c r="J117" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" ht="14.25">
       <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
-      <c r="C118" s="4" t="s">
-        <v>139</v>
-      </c>
+      <c r="B118" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
-      <c r="H118" s="4"/>
+      <c r="H118" s="17"/>
       <c r="I118" s="6"/>
-      <c r="J118" s="9" t="s">
+      <c r="J118" s="18"/>
+    </row>
+    <row r="119" ht="28.5">
+      <c r="C119" t="s">
+        <v>139</v>
+      </c>
+      <c r="I119" s="6"/>
+      <c r="J119" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="119" ht="28.5">
-      <c r="A119" s="4"/>
-      <c r="B119" s="4" t="s">
+    <row r="120" ht="28.5">
+      <c r="B120" t="s">
         <v>141</v>
       </c>
-      <c r="C119" s="4"/>
-      <c r="D119" s="4"/>
-      <c r="E119" s="4"/>
-      <c r="F119" s="4"/>
-      <c r="G119" s="4"/>
-      <c r="H119" s="16"/>
-      <c r="I119" s="6"/>
-      <c r="J119" s="17"/>
-    </row>
-    <row r="120" ht="28.5">
-      <c r="C120" t="s">
+      <c r="C120" s="19"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="19"/>
+    </row>
+    <row r="121" ht="28.5">
+      <c r="C121" t="s">
         <v>142</v>
       </c>
-      <c r="I120" s="6"/>
-      <c r="J120" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="121" ht="28.5">
-      <c r="B121" t="s">
-        <v>144</v>
-      </c>
-      <c r="C121" s="18"/>
       <c r="I121" s="6"/>
-      <c r="J121" s="18"/>
     </row>
     <row r="122" ht="14.25">
       <c r="C122" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I122" s="6"/>
     </row>
     <row r="123" ht="14.25">
       <c r="C123" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="I123" s="6"/>
     </row>
-    <row r="124" ht="14.25">
-      <c r="C124" t="s">
-        <v>95</v>
-      </c>
-      <c r="I124" s="6"/>
-    </row>
+    <row r="124" ht="14.25"/>
     <row r="125" ht="28.5"/>
     <row r="126" ht="14.25"/>
     <row r="127" ht="14.25"/>
@@ -3153,7 +3136,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00140028-0061-4081-939A-003200B60096}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00CF00A0-0018-45A4-8E51-0009004B00E1}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3167,27 +3150,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I102 I104:I115 I46:I49</xm:sqref>
+          <xm:sqref>I3:I101 I103:I114 I45:I48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00F600E3-0084-452B-8C50-007B00F1003C}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I117</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00500018-000F-42F2-BFAD-006E00C400DB}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00780089-00B1-476C-A9AE-00350015009D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3204,7 +3170,7 @@
           <xm:sqref>I116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00590088-0043-40EE-BB7E-009B00D60066}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0048005C-008E-4A5E-A057-00D4008A00F6}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3218,10 +3184,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I28</xm:sqref>
+          <xm:sqref>I115</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007F003B-00F2-4457-A389-0097001F00B6}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{000600AB-00FC-45E0-BAAD-0045005F0031}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3238,7 +3204,24 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E100FC-0003-4B0B-BE01-007A006C0006}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00AE004D-00E1-417D-80FF-00EE009F0074}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I26</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00F100DD-0032-4F61-8818-00B70024004B}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3255,7 +3238,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00D300D9-00F2-460D-900F-006200DE0076}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00B3003A-007C-46DF-8DAE-008C00220027}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3269,27 +3252,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I44</xm:sqref>
+          <xm:sqref>I43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{005E00A4-004D-4401-8A55-00EE006B0088}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="7" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I69</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00BD0074-0038-4BB1-8561-00C3005B00A6}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{008C0006-005C-4EEC-A4EF-00DF009D00DA}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3306,7 +3272,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00E00024-00E9-468A-8E3C-000B00CC009A}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00480027-0006-48A1-B2FF-002300ED001D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3323,7 +3289,41 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00ED00D2-002C-4B20-82E1-00F1002E0014}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00670048-00C2-49BD-BB74-00520041000B}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I66</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{009D0059-0069-4721-BCD8-0068001900A3}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I118</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0053000B-00ED-4F52-9D29-00E500CA0049}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3340,7 +3340,24 @@
           <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00BA0062-00E0-47A6-BEBA-002600C80027}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00240055-00CF-44FA-A659-004F00FF0045}">
+            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="7" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I102</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{006100F2-00A7-4967-92CE-00AE00320043}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3357,41 +3374,92 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{005500F9-0079-4C76-972D-0060003200CC}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+          <x14:cfRule type="containsText" priority="3" text="1" id="{008D00E0-009F-470A-A9E2-000F003700D2}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
-                <color theme="7" tint="0.79998168889431442"/>
+                <color theme="9" tint="0.79998168889431442"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I103</xm:sqref>
+          <xm:sqref>I26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{007C0082-007C-468F-A80C-00D500D8005E}">
-            <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00E200E3-00F8-4BFA-AC63-000200B100E5}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
-                <color theme="7" tint="0.79998168889431442"/>
+                <color theme="9" tint="0.79998168889431442"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC000"/>
-                  <bgColor rgb="FFFFC000"/>
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I121</xm:sqref>
+          <xm:sqref>I116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0025002C-0006-4A12-B027-00C4007E001D}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00CA0000-0083-446F-9114-001B009B0055}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I3:I101 I103:I114 I45:I48</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00670002-0029-4547-9129-007400C0005D}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I2</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000C00F8-0065-4684-84CF-002A0043001C}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I115</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C100B5-00C4-4DCC-8FA3-00DC00190016}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3408,7 +3476,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00F700EA-0046-4CC5-BDB7-00EC00B600AB}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00C3004F-006C-48E7-9D37-002F008A00B3}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3422,112 +3490,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I117</xm:sqref>
+          <xm:sqref>I43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00CF00F2-00FE-4090-AAF0-0013006B0092}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I3:I102 I104:I115 I46:I49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003C003F-0006-4E03-AA78-0081005A00BC}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0003000F-00C8-4ECD-A3EA-0082009400F9}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I116</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{009C0065-00C5-4846-A053-00E800FD007D}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B40088-000F-45E6-86B5-008600D0005F}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I44</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00A90082-00CD-43CC-A887-00B60018001B}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I69</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{001000A2-00BA-4938-9E32-00D400380010}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{000100A1-0092-4845-AD92-004C00B300BF}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3544,7 +3510,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{003200FB-00A6-4311-B395-00C100650003}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00A100C9-0002-4976-B1AB-0060000700E9}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3561,7 +3527,41 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{008A00E2-00F3-4E60-A483-00610027009A}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{007900AA-009B-41B0-B7F4-001B00C90044}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I66</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0096006B-00D0-484C-A8CD-0032009300C9}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I118</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00B800F6-0028-4149-930D-00DD00D300D3}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3578,7 +3578,24 @@
           <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00490074-001A-42D3-A940-001D00DC00E2}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D4007A-00BF-47C7-887C-005A004900A1}">
+            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="9" tint="0.79998168889431442"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF00B050"/>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>I102</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{009100EA-00C3-488E-8A5B-0068008A00D7}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3595,41 +3612,7 @@
           <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00D3000E-0024-4D3B-9307-0062003400CA}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I103</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{004000D3-0031-4A0E-B888-002000B600A6}">
-            <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="9" tint="0.79998168889431442"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF00B050"/>
-                  <bgColor rgb="FF00B050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>I121</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00DC002A-00F4-4FE6-B262-004B003900AD}">
+          <x14:cfRule type="dataBar" priority="2" id="{00CB007B-00F8-4C85-85DB-00CD008000FE}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3645,7 +3628,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{00A7003C-0034-4A00-A7AD-005E006C007B}">
+          <x14:cfRule type="dataBar" priority="1" id="{0013002A-0035-433B-A0A2-00D000E800FF}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
fixed mission location save bug
</commit_message>
<xml_diff>
--- a/SatManager Work Breakdown Structure.xlsx
+++ b/SatManager Work Breakdown Structure.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>Status</t>
   </si>
@@ -408,13 +408,25 @@
     <t xml:space="preserve">pause menu</t>
   </si>
   <si>
+    <t xml:space="preserve">escape to bring up</t>
+  </si>
+  <si>
     <t>save</t>
   </si>
   <si>
+    <t xml:space="preserve">satellite list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mission list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orbit path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mission transforms changing</t>
+  </si>
+  <si>
     <t>settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">return to main menu</t>
   </si>
   <si>
     <t xml:space="preserve">Graphics rework</t>
@@ -588,7 +600,7 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="44" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -630,12 +642,6 @@
     <xf fontId="2" fillId="3" borderId="3" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -663,7 +669,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J123" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Table5" ref="A2:J126" headerRowCount="0">
   <tableColumns count="10">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1173,7 +1179,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A94" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1227,13 +1233,13 @@
       <c r="J2" s="7"/>
       <c r="L2" s="8">
         <f>SUM(Table5[Status])/ROWS(Table5[])</f>
-        <v>0.52459016393442626</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
-        <f>COUNTIF(I2:I114,"0")/ROWS(Table5[])</f>
-        <v>1.6393442622950821e-002</v>
+        <f>COUNTIF(I2:I117,"0")/ROWS(Table5[])</f>
+        <v>2.4e-002</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -1249,9 +1255,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
+      <c r="I3" s="6"/>
       <c r="J3" s="9"/>
       <c r="L3" t="s">
         <v>6</v>
@@ -1268,13 +1272,11 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
+      <c r="I4" s="6"/>
       <c r="J4" s="9"/>
       <c r="L4">
         <f>ROWS(Table5[])</f>
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1309,7 +1311,7 @@
       <c r="J6" s="9"/>
       <c r="L6">
         <f>SUM(Table5[Status])</f>
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -2340,22 +2342,24 @@
     <row r="71" ht="14.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="15"/>
+      <c r="C71" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D71" s="4"/>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="6"/>
-      <c r="J71" s="16"/>
+      <c r="J71" s="9"/>
     </row>
     <row r="72" ht="14.25">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
-      <c r="C72" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -2367,10 +2371,10 @@
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
@@ -2383,7 +2387,7 @@
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -2395,10 +2399,10 @@
       <c r="A75" s="4"/>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4" t="s">
-        <v>100</v>
-      </c>
+      <c r="D75" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
@@ -2409,10 +2413,10 @@
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
-      <c r="D76" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
@@ -2425,7 +2429,7 @@
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
@@ -2439,7 +2443,7 @@
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
@@ -2451,10 +2455,10 @@
       <c r="A79" s="4"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="D79" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="4"/>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
@@ -2465,10 +2469,10 @@
       <c r="A80" s="4"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
-      <c r="D80" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
@@ -2481,7 +2485,7 @@
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -2492,24 +2496,26 @@
     <row r="82" ht="14.25">
       <c r="A82" s="4"/>
       <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
+      <c r="C82" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="D82" s="4"/>
-      <c r="E82" s="4" t="s">
-        <v>105</v>
-      </c>
+      <c r="E82" s="4"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
-      <c r="I82" s="6"/>
+      <c r="I82" s="6">
+        <v>1</v>
+      </c>
       <c r="J82" s="9"/>
     </row>
     <row r="83" ht="14.25">
       <c r="A83" s="4"/>
       <c r="B83" s="4"/>
-      <c r="C83" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D83" s="4"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
@@ -2517,14 +2523,16 @@
       <c r="I83" s="6">
         <v>1</v>
       </c>
-      <c r="J83" s="9"/>
+      <c r="J83" s="9" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="84" ht="14.25">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
@@ -2534,36 +2542,34 @@
         <v>1</v>
       </c>
       <c r="J84" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" ht="14.25">
       <c r="A85" s="4"/>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
-      <c r="D85" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E85" s="4"/>
+      <c r="D85" s="4"/>
+      <c r="E85" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
       <c r="I85" s="6">
         <v>1</v>
       </c>
-      <c r="J85" s="9" t="s">
-        <v>110</v>
-      </c>
+      <c r="J85" s="9"/>
     </row>
     <row r="86" ht="14.25">
       <c r="A86" s="4"/>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
-      <c r="E86" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F86" s="4"/>
+      <c r="E86" s="4"/>
+      <c r="F86" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="6">
@@ -2578,7 +2584,7 @@
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
       <c r="F87" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
@@ -2594,7 +2600,7 @@
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
       <c r="F88" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
@@ -2610,7 +2616,7 @@
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
@@ -2624,34 +2630,34 @@
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
-      <c r="E90" s="4"/>
-      <c r="F90" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="E90" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F90" s="4"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="6">
         <v>1</v>
       </c>
-      <c r="J90" s="9"/>
+      <c r="J90" s="9" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="91" ht="14.25">
       <c r="A91" s="4"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
-      <c r="E91" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F91" s="4"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="6">
         <v>1</v>
       </c>
-      <c r="J91" s="9" t="s">
-        <v>116</v>
-      </c>
+      <c r="J91" s="9"/>
     </row>
     <row r="92" ht="14.25">
       <c r="A92" s="4"/>
@@ -2660,7 +2666,7 @@
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
       <c r="F92" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
@@ -2676,7 +2682,7 @@
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
       <c r="F93" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
@@ -2692,7 +2698,7 @@
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
@@ -2706,10 +2712,10 @@
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
-      <c r="E95" s="4"/>
-      <c r="F95" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="E95" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F95" s="4"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="6">
@@ -2722,10 +2728,10 @@
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
-      <c r="E96" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F96" s="4"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="6">
@@ -2740,14 +2746,16 @@
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="6">
         <v>1</v>
       </c>
-      <c r="J97" s="9"/>
+      <c r="J97" s="9" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="98" ht="14.25">
       <c r="A98" s="4"/>
@@ -2756,16 +2764,14 @@
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
       <c r="F98" s="4" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="6">
         <v>1</v>
       </c>
-      <c r="J98" s="9" t="s">
-        <v>122</v>
-      </c>
+      <c r="J98" s="9"/>
     </row>
     <row r="99" ht="14.25">
       <c r="A99" s="4"/>
@@ -2774,7 +2780,7 @@
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
@@ -2787,11 +2793,11 @@
       <c r="A100" s="4"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
-      <c r="D100" s="4"/>
+      <c r="D100" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="E100" s="4"/>
-      <c r="F100" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="F100" s="4"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="6">
@@ -2803,10 +2809,10 @@
       <c r="A101" s="4"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
-      <c r="D101" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
@@ -2821,7 +2827,7 @@
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
@@ -2836,10 +2842,10 @@
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
-      <c r="E103" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="F103" s="4"/>
+      <c r="E103" s="4"/>
+      <c r="F103" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="6">
@@ -2854,7 +2860,7 @@
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
       <c r="F104" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
@@ -2868,9 +2874,8 @@
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
-      <c r="E105" s="4"/>
       <c r="F105" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
@@ -2883,10 +2888,11 @@
       <c r="A106" s="4"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
-      <c r="F106" s="4" t="s">
-        <v>127</v>
-      </c>
+      <c r="D106" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E106" s="4"/>
+      <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="6">
@@ -2898,10 +2904,10 @@
       <c r="A107" s="4"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
-      <c r="D107" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
@@ -2916,7 +2922,7 @@
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="E108" s="4" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="F108" s="4"/>
       <c r="G108" s="4"/>
@@ -2929,31 +2935,33 @@
     <row r="109" ht="14.25">
       <c r="A109" s="4"/>
       <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
+      <c r="C109" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="D109" s="4"/>
-      <c r="E109" s="4" t="s">
-        <v>129</v>
-      </c>
+      <c r="E109" s="4"/>
       <c r="F109" s="4"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J109" s="9"/>
     </row>
     <row r="110" ht="14.25">
       <c r="A110" s="4"/>
       <c r="B110" s="4"/>
-      <c r="C110" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="D110" s="4"/>
+      <c r="C110" s="4"/>
+      <c r="D110" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="E110" s="4"/>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
-      <c r="I110" s="6"/>
+      <c r="I110" s="6">
+        <v>1</v>
+      </c>
       <c r="J110" s="9"/>
     </row>
     <row r="111" ht="14.25">
@@ -2961,37 +2969,41 @@
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E111" s="4"/>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
-      <c r="I111" s="6"/>
+      <c r="I111" s="6">
+        <v>0</v>
+      </c>
       <c r="J111" s="9"/>
     </row>
     <row r="112" ht="14.25">
       <c r="A112" s="4"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
-      <c r="D112" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="F112" s="4"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
-      <c r="I112" s="6"/>
+      <c r="I112" s="6">
+        <v>0</v>
+      </c>
       <c r="J112" s="9"/>
     </row>
     <row r="113" ht="14.25">
       <c r="A113" s="4"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
-      <c r="D113" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="F113" s="4"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
@@ -3002,10 +3014,10 @@
       <c r="A114" s="4"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
-      <c r="D114" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
@@ -3014,49 +3026,47 @@
     </row>
     <row r="115" ht="14.25">
       <c r="A115" s="4"/>
-      <c r="B115" s="4" t="s">
-        <v>134</v>
-      </c>
+      <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
-      <c r="E115" s="4"/>
+      <c r="E115" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
-      <c r="I115" s="6"/>
+      <c r="I115" s="6">
+        <v>1</v>
+      </c>
       <c r="J115" s="9"/>
     </row>
     <row r="116" ht="14.25">
       <c r="A116" s="4"/>
       <c r="B116" s="4"/>
-      <c r="C116" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D116" s="4"/>
+      <c r="C116" s="4"/>
+      <c r="D116" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
       <c r="I116" s="6"/>
-      <c r="J116" s="9" t="s">
-        <v>135</v>
-      </c>
+      <c r="J116" s="9"/>
     </row>
     <row r="117" ht="14.25">
       <c r="A117" s="4"/>
       <c r="B117" s="4"/>
-      <c r="C117" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D117" s="4"/>
+      <c r="C117" s="4"/>
+      <c r="D117" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="6"/>
-      <c r="J117" s="9" t="s">
-        <v>137</v>
-      </c>
+      <c r="J117" s="9"/>
     </row>
     <row r="118" ht="14.25">
       <c r="A118" s="4"/>
@@ -3068,56 +3078,102 @@
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
-      <c r="H118" s="17"/>
+      <c r="H118" s="4"/>
       <c r="I118" s="6"/>
-      <c r="J118" s="18"/>
-    </row>
-    <row r="119" ht="28.5">
-      <c r="C119" t="s">
+      <c r="J118" s="9"/>
+    </row>
+    <row r="119" ht="14.25">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D119" s="4"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="4"/>
+      <c r="G119" s="4"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="6"/>
+      <c r="J119" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="I119" s="6"/>
-      <c r="J119" s="1" t="s">
+    </row>
+    <row r="120" ht="14.25">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="120" ht="28.5">
-      <c r="B120" t="s">
+      <c r="D120" s="4"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="4"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="4"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="C120" s="19"/>
-      <c r="I120" s="6"/>
-      <c r="J120" s="19"/>
-    </row>
-    <row r="121" ht="28.5">
-      <c r="C121" t="s">
+    </row>
+    <row r="121" ht="14.25">
+      <c r="A121" s="4"/>
+      <c r="B121" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="15"/>
       <c r="I121" s="6"/>
-    </row>
-    <row r="122" ht="14.25">
+      <c r="J121" s="16"/>
+    </row>
+    <row r="122" ht="28.5">
       <c r="C122" t="s">
         <v>143</v>
       </c>
       <c r="I122" s="6"/>
-    </row>
-    <row r="123" ht="14.25">
-      <c r="C123" t="s">
+      <c r="J122" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="123" ht="28.5">
+      <c r="B123" t="s">
+        <v>145</v>
+      </c>
+      <c r="C123" s="17"/>
+      <c r="I123" s="6"/>
+      <c r="J123" s="17"/>
+    </row>
+    <row r="124" ht="28.5">
+      <c r="C124" t="s">
+        <v>146</v>
+      </c>
+      <c r="I124" s="6"/>
+    </row>
+    <row r="125" ht="14.25">
+      <c r="C125" t="s">
+        <v>147</v>
+      </c>
+      <c r="I125" s="6"/>
+    </row>
+    <row r="126" ht="14.25">
+      <c r="C126" t="s">
         <v>94</v>
       </c>
-      <c r="I123" s="6"/>
-    </row>
-    <row r="124" ht="14.25"/>
-    <row r="125" ht="28.5"/>
-    <row r="126" ht="14.25"/>
+      <c r="I126" s="6"/>
+    </row>
     <row r="127" ht="14.25"/>
-    <row r="128" ht="14.25"/>
+    <row r="128" ht="28.5"/>
     <row r="129" ht="14.25"/>
     <row r="130" ht="14.25"/>
     <row r="131" ht="14.25"/>
     <row r="132" ht="14.25"/>
     <row r="133" ht="14.25"/>
     <row r="134" ht="14.25"/>
+    <row r="135" ht="14.25"/>
+    <row r="136" ht="14.25"/>
+    <row r="137" ht="14.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="L1:M1"/>
@@ -3136,7 +3192,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00CF00A0-0018-45A4-8E51-0009004B00E1}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00BC00A1-0059-480E-A4EE-00D400F20046}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3150,10 +3206,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I101 I103:I114 I45:I48</xm:sqref>
+          <xm:sqref>I3:I100 I102:I117 I45:I48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00780089-00B1-476C-A9AE-00350015009D}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{000800EF-0064-47F0-8110-007B001C0043}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3167,10 +3223,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I116</xm:sqref>
+          <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0048005C-008E-4A5E-A057-00D4008A00F6}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{002A0057-000D-4C9F-8608-007A000E003D}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3184,10 +3240,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I115</xm:sqref>
+          <xm:sqref>I118</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{000600AB-00FC-45E0-BAAD-0045005F0031}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E3006E-004C-41F2-B811-00960009004C}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3204,7 +3260,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00AE004D-00E1-417D-80FF-00EE009F0074}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{0069004C-00F0-4D25-8D96-00D400DF00A8}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3221,7 +3277,7 @@
           <xm:sqref>I26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00F100DD-0032-4F61-8818-00B70024004B}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00E8000F-001A-4F57-A3B7-00000077002F}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3238,7 +3294,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00B3003A-007C-46DF-8DAE-008C00220027}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00FC0056-00BD-480D-82C8-0027004D00E4}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3255,7 +3311,7 @@
           <xm:sqref>I43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{008C0006-005C-4EEC-A4EF-00DF009D00DA}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003800C7-0024-47AD-B2D1-001D00EF006B}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3272,7 +3328,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00480027-0006-48A1-B2FF-002300ED001D}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00A20089-006C-4204-A010-00F80081008E}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3289,7 +3345,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00670048-00C2-49BD-BB74-00520041000B}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{003400CA-0006-40C1-8F71-0093003900BA}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3306,7 +3362,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{009D0059-0069-4721-BCD8-0068001900A3}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{005D003B-0037-45F8-A31D-000D00E30083}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3320,10 +3376,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I118</xm:sqref>
+          <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{0053000B-00ED-4F52-9D29-00E500CA0049}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{007E008F-0097-4EA0-AEE9-0047005F001C}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3337,10 +3393,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I119</xm:sqref>
+          <xm:sqref>I122</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{00240055-00CF-44FA-A659-004F00FF0045}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{006E00FF-0095-4515-9CE3-0069001E00DF}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3354,10 +3410,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I102</xm:sqref>
+          <xm:sqref>I101</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" text="0" id="{006100F2-00A7-4967-92CE-00AE00320043}">
+          <x14:cfRule type="containsText" priority="4" text="0" id="{00F600C9-00F1-4396-A1CA-005E00A800CB}">
             <xm:f>NOT(ISERROR(SEARCH("0",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3371,10 +3427,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I120</xm:sqref>
+          <xm:sqref>I123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{008D00E0-009F-470A-A9E2-000F003700D2}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{005500AD-0041-46C8-8192-005300190001}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3391,7 +3447,7 @@
           <xm:sqref>I26</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00E200E3-00F8-4BFA-AC63-000200B100E5}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00BD006E-006D-4031-A3E3-003C00A00047}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3405,10 +3461,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I116</xm:sqref>
+          <xm:sqref>I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00CA0000-0083-446F-9114-001B009B0055}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00D50057-0033-48BE-B89A-004F00FF0085}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3422,10 +3478,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I3:I101 I103:I114 I45:I48</xm:sqref>
+          <xm:sqref>I3:I100 I102:I117 I45:I48</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00670002-0029-4547-9129-007400C0005D}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{003500B4-00A3-433E-AC45-0086000E004B}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3442,7 +3498,7 @@
           <xm:sqref>I2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000C00F8-0065-4684-84CF-002A0043001C}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00ED0054-00A4-4EE5-ACAB-002200370048}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3456,10 +3512,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I115</xm:sqref>
+          <xm:sqref>I118</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C100B5-00C4-4DCC-8FA3-00DC00190016}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00FE000E-006D-49CA-BD44-002300FB00D4}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3476,7 +3532,7 @@
           <xm:sqref>I27</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00C3004F-006C-48E7-9D37-002F008A00B3}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00DF0039-000D-4369-9BB9-00D1006C0067}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3493,7 +3549,7 @@
           <xm:sqref>I43</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{000100A1-0092-4845-AD92-004C00B300BF}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00FA0032-00E4-4F22-B46F-003600B10020}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3510,7 +3566,7 @@
           <xm:sqref>I68</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00A100C9-0002-4976-B1AB-0060000700E9}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{002C00D9-0028-46B7-A6F4-00A10085003F}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3527,7 +3583,7 @@
           <xm:sqref>I67</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{007900AA-009B-41B0-B7F4-001B00C90044}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00480014-0061-4CD2-9A95-002400B800AB}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3544,7 +3600,7 @@
           <xm:sqref>I66</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{0096006B-00D0-484C-A8CD-0032009300C9}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{0095004B-00EC-4F7D-A2CD-001700AC006D}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3558,10 +3614,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I118</xm:sqref>
+          <xm:sqref>I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00B800F6-0028-4149-930D-00DD00D300D3}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{004C00EB-007C-4AA8-B3CB-009400DA0033}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3575,10 +3631,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I119</xm:sqref>
+          <xm:sqref>I122</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{00D4007A-00BF-47C7-887C-005A004900A1}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{001B00E4-0094-4AA7-A6F3-00F9004B00CE}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3592,10 +3648,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I102</xm:sqref>
+          <xm:sqref>I101</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" text="1" id="{009100EA-00C3-488E-8A5B-0068008A00D7}">
+          <x14:cfRule type="containsText" priority="3" text="1" id="{00A4002B-000F-4EB1-8F5F-0069001F00B4}">
             <xm:f>NOT(ISERROR(SEARCH("1",I2)))</xm:f>
             <x14:dxf>
               <font>
@@ -3609,10 +3665,10 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>I120</xm:sqref>
+          <xm:sqref>I123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="2" id="{00CB007B-00F8-4C85-85DB-00CD008000FE}">
+          <x14:cfRule type="dataBar" priority="2" id="{00FE0038-0098-4B62-9E5A-004A0009007F}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -3628,7 +3684,7 @@
           <xm:sqref>L2</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" priority="1" id="{0013002A-0035-433B-A0A2-00D000E800FF}">
+          <x14:cfRule type="dataBar" priority="1" id="{00330088-0032-4D39-97E3-00C800D0006C}">
             <x14:dataBar maxLength="100" minLength="0" axisPosition="automatic" direction="context" gradient="0" negativeBarColorSameAsPositive="1">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>